<commit_message>
Add phone number validation and filter for specialty in data processing
</commit_message>
<xml_diff>
--- a/NV.xlsx
+++ b/NV.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Y64"/>
+  <dimension ref="A1:Y53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -566,7 +566,7 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>45967.57631624236</v>
+        <v>45967.7930625937</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -596,8 +596,10 @@
           <t>ORFELINA DEL CARMEN CACERES SUAREZ</t>
         </is>
       </c>
-      <c r="H2" t="n">
-        <v>3147588813</v>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>3147588813</t>
+        </is>
       </c>
       <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr">
@@ -651,7 +653,7 @@
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>45967.57631624448</v>
+        <v>45967.79306260568</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -674,17 +676,23 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>1063294951</v>
+        <v>78585766</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>DAYANA ISABEL REGINO MADERA</t>
-        </is>
-      </c>
-      <c r="H3" t="n">
-        <v>3164600121</v>
-      </c>
-      <c r="I3" t="inlineStr"/>
+          <t>FRANCISCO MANUEL FLOREZ MARTINEZ</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>3148434454</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>3148434454</t>
+        </is>
+      </c>
       <c r="J3" t="inlineStr">
         <is>
           <t>05/11/2025</t>
@@ -692,35 +700,35 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>Z300</t>
+          <t>K769</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>GIOVANINA  BLANQUISETT BELLO</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr"/>
+          <t>CARLOS FEDERICO AYALA PALENCIA</t>
+        </is>
+      </c>
+      <c r="M3" t="n">
+        <v>78</v>
+      </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>PYP MEDICO</t>
+          <t>MEDICINA GENERAL</t>
         </is>
       </c>
       <c r="O3" t="n">
-        <v>906039</v>
+        <v>902206</v>
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>TREPONEMA PALLIDUM  - Prueba Rapida</t>
+          <t>EXTENDIDO DE SANGRE PERIFERICA  ESTUDIO DE MORFOLOGIA</t>
         </is>
       </c>
       <c r="Q3" t="n">
         <v>1</v>
       </c>
       <c r="R3" t="inlineStr"/>
-      <c r="S3" t="n">
-        <v>0</v>
-      </c>
+      <c r="S3" t="inlineStr"/>
       <c r="T3" t="inlineStr"/>
       <c r="U3" t="inlineStr"/>
       <c r="V3" t="inlineStr"/>
@@ -734,7 +742,7 @@
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
-        <v>45967.57631624544</v>
+        <v>45967.79306260568</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -757,17 +765,23 @@
         </is>
       </c>
       <c r="F4" t="n">
-        <v>1063294951</v>
+        <v>78585766</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>DAYANA ISABEL REGINO MADERA</t>
-        </is>
-      </c>
-      <c r="H4" t="n">
-        <v>3164600121</v>
-      </c>
-      <c r="I4" t="inlineStr"/>
+          <t>FRANCISCO MANUEL FLOREZ MARTINEZ</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>3148434454</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>3148434454</t>
+        </is>
+      </c>
       <c r="J4" t="inlineStr">
         <is>
           <t>05/11/2025</t>
@@ -775,35 +789,35 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>Z300</t>
+          <t>K769</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>GIOVANINA  BLANQUISETT BELLO</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr"/>
+          <t>CARLOS FEDERICO AYALA PALENCIA</t>
+        </is>
+      </c>
+      <c r="M4" t="n">
+        <v>78</v>
+      </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>PYP MEDICO</t>
+          <t>MEDICINA GENERAL</t>
         </is>
       </c>
       <c r="O4" t="n">
-        <v>906249</v>
+        <v>903809</v>
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>VIH 1 Y 2  ANTICUERPOS PRUEBA RAPIDA</t>
+          <t>BILIRRUBINAS TOTAL Y DIRECTA</t>
         </is>
       </c>
       <c r="Q4" t="n">
         <v>1</v>
       </c>
       <c r="R4" t="inlineStr"/>
-      <c r="S4" t="n">
-        <v>0</v>
-      </c>
+      <c r="S4" t="inlineStr"/>
       <c r="T4" t="inlineStr"/>
       <c r="U4" t="inlineStr"/>
       <c r="V4" t="inlineStr"/>
@@ -817,7 +831,7 @@
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
-        <v>45967.5763162463</v>
+        <v>45967.79306260568</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -836,23 +850,25 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>RC</t>
+          <t>CC</t>
         </is>
       </c>
       <c r="F5" t="n">
-        <v>1066577109</v>
+        <v>78585766</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>SAMUEL  CAMARGO RAMOS</t>
-        </is>
-      </c>
-      <c r="H5" t="n">
-        <v>3117442626</v>
+          <t>FRANCISCO MANUEL FLOREZ MARTINEZ</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>3148434454</t>
+        </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>3022136815</t>
+          <t>3148434454</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
@@ -862,35 +878,35 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>Z001</t>
+          <t>K769</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>PAULA ANDREA AGUAS VERGARA</t>
-        </is>
-      </c>
-      <c r="M5" t="inlineStr"/>
+          <t>CARLOS FEDERICO AYALA PALENCIA</t>
+        </is>
+      </c>
+      <c r="M5" t="n">
+        <v>78</v>
+      </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>PYP ENFERMERIA</t>
+          <t>MEDICINA GENERAL</t>
         </is>
       </c>
       <c r="O5" t="n">
-        <v>194140</v>
+        <v>903833</v>
       </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>MÉDICO U ODONTÓLOGO GENERAL</t>
+          <t>FOSFATASA ALCALINA</t>
         </is>
       </c>
       <c r="Q5" t="n">
         <v>1</v>
       </c>
       <c r="R5" t="inlineStr"/>
-      <c r="S5" t="n">
-        <v>0</v>
-      </c>
+      <c r="S5" t="inlineStr"/>
       <c r="T5" t="inlineStr"/>
       <c r="U5" t="inlineStr"/>
       <c r="V5" t="inlineStr"/>
@@ -904,7 +920,7 @@
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
-        <v>45967.57631624712</v>
+        <v>45967.79306260568</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -934,8 +950,10 @@
           <t>FRANCISCO MANUEL FLOREZ MARTINEZ</t>
         </is>
       </c>
-      <c r="H6" t="n">
-        <v>3148434454</v>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>3148434454</t>
+        </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
@@ -966,11 +984,11 @@
         </is>
       </c>
       <c r="O6" t="n">
-        <v>902206</v>
+        <v>903866</v>
       </c>
       <c r="P6" t="inlineStr">
         <is>
-          <t>EXTENDIDO DE SANGRE PERIFERICA  ESTUDIO DE MORFOLOGIA</t>
+          <t>TRANSAMINASA GLUTÁMICOPIRÚVICA O ALANINO AMINO TRANSFE-RASA TGP-ALT *</t>
         </is>
       </c>
       <c r="Q6" t="n">
@@ -991,7 +1009,7 @@
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
-        <v>45967.57631624794</v>
+        <v>45967.79306260568</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -1021,8 +1039,10 @@
           <t>FRANCISCO MANUEL FLOREZ MARTINEZ</t>
         </is>
       </c>
-      <c r="H7" t="n">
-        <v>3148434454</v>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>3148434454</t>
+        </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
@@ -1053,11 +1073,11 @@
         </is>
       </c>
       <c r="O7" t="n">
-        <v>903809</v>
+        <v>903867</v>
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>BILIRRUBINAS TOTAL Y DIRECTA</t>
+          <t>TRANSAMINASA GLUTÁMICO OXALACÉTICA O ASPARTATO AMINO TRANSFERASA TGO-AST</t>
         </is>
       </c>
       <c r="Q7" t="n">
@@ -1078,7 +1098,7 @@
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
-        <v>45967.57631624875</v>
+        <v>45967.79306260568</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -1101,19 +1121,21 @@
         </is>
       </c>
       <c r="F8" t="n">
-        <v>78585766</v>
+        <v>25991655</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>FRANCISCO MANUEL FLOREZ MARTINEZ</t>
-        </is>
-      </c>
-      <c r="H8" t="n">
-        <v>3148434454</v>
+          <t>MARTHA ELENA CALLE CONTRERAS</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>3138983159</t>
+        </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>3148434454</t>
+          <t>3008196562</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
@@ -1123,12 +1145,12 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>K769</t>
+          <t>M624</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>CARLOS FEDERICO AYALA PALENCIA</t>
+          <t>EDGAR  EMBUZ TORRALVO</t>
         </is>
       </c>
       <c r="M8" t="n">
@@ -1140,18 +1162,20 @@
         </is>
       </c>
       <c r="O8" t="n">
-        <v>903833</v>
+        <v>931001</v>
       </c>
       <c r="P8" t="inlineStr">
         <is>
-          <t>FOSFATASA ALCALINA</t>
+          <t>TERAPIA FISICA INTEGRAL SOD</t>
         </is>
       </c>
       <c r="Q8" t="n">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="R8" t="inlineStr"/>
-      <c r="S8" t="inlineStr"/>
+      <c r="S8" t="n">
+        <v>0</v>
+      </c>
       <c r="T8" t="inlineStr"/>
       <c r="U8" t="inlineStr"/>
       <c r="V8" t="inlineStr"/>
@@ -1165,7 +1189,7 @@
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
-        <v>45967.57631624956</v>
+        <v>45967.79306260568</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -1188,19 +1212,21 @@
         </is>
       </c>
       <c r="F9" t="n">
-        <v>78585766</v>
+        <v>50941982</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>FRANCISCO MANUEL FLOREZ MARTINEZ</t>
-        </is>
-      </c>
-      <c r="H9" t="n">
-        <v>3148434454</v>
+          <t>NORMA DE JESUS RIVERO ARROYO</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>3137379666</t>
+        </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>3148434454</t>
+          <t>3145447973</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
@@ -1210,12 +1236,12 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>K769</t>
+          <t>K580</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>CARLOS FEDERICO AYALA PALENCIA</t>
+          <t>MAIRON ALDAHIR ANGULO CARVAJAL</t>
         </is>
       </c>
       <c r="M9" t="n">
@@ -1227,18 +1253,20 @@
         </is>
       </c>
       <c r="O9" t="n">
-        <v>903866</v>
+        <v>452301</v>
       </c>
       <c r="P9" t="inlineStr">
         <is>
-          <t>TRANSAMINASA GLUTÁMICOPIRÚVICA O ALANINO AMINO TRANSFE-RASA TGP-ALT *</t>
+          <t>COLONOSCOPIA TOTAL</t>
         </is>
       </c>
       <c r="Q9" t="n">
         <v>1</v>
       </c>
       <c r="R9" t="inlineStr"/>
-      <c r="S9" t="inlineStr"/>
+      <c r="S9" t="n">
+        <v>0</v>
+      </c>
       <c r="T9" t="inlineStr"/>
       <c r="U9" t="inlineStr"/>
       <c r="V9" t="inlineStr"/>
@@ -1252,7 +1280,7 @@
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">
-        <v>45967.57631625037</v>
+        <v>45967.79306261727</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -1275,19 +1303,21 @@
         </is>
       </c>
       <c r="F10" t="n">
-        <v>78585766</v>
+        <v>25987708</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>FRANCISCO MANUEL FLOREZ MARTINEZ</t>
-        </is>
-      </c>
-      <c r="H10" t="n">
-        <v>3148434454</v>
+          <t>ALBA ROSA PEÑA BURGOS</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>3147707175</t>
+        </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>3148434454</t>
+          <t>3147707175</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
@@ -1297,12 +1327,12 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>K769</t>
+          <t>Z712</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>CARLOS FEDERICO AYALA PALENCIA</t>
+          <t>YEIDIS PATRICIA LOPEZ  BRAVO</t>
         </is>
       </c>
       <c r="M10" t="n">
@@ -1314,18 +1344,20 @@
         </is>
       </c>
       <c r="O10" t="n">
-        <v>903867</v>
+        <v>881332</v>
       </c>
       <c r="P10" t="inlineStr">
         <is>
-          <t>TRANSAMINASA GLUTÁMICO OXALACÉTICA O ASPARTATO AMINO TRANSFERASA TGO-AST</t>
+          <t>ULTRASONOGRAFIA DE VÍAS URINARIAS (RIÑONES  VEJIGA Y PROSTATA TRANSABDOMINAL)</t>
         </is>
       </c>
       <c r="Q10" t="n">
         <v>1</v>
       </c>
       <c r="R10" t="inlineStr"/>
-      <c r="S10" t="inlineStr"/>
+      <c r="S10" t="n">
+        <v>0</v>
+      </c>
       <c r="T10" t="inlineStr"/>
       <c r="U10" t="inlineStr"/>
       <c r="V10" t="inlineStr"/>
@@ -1339,7 +1371,7 @@
     </row>
     <row r="11">
       <c r="A11" s="2" t="n">
-        <v>45967.5763162512</v>
+        <v>45967.79306261727</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
@@ -1362,19 +1394,21 @@
         </is>
       </c>
       <c r="F11" t="n">
-        <v>25991655</v>
+        <v>1040491654</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>MARTHA ELENA CALLE CONTRERAS</t>
-        </is>
-      </c>
-      <c r="H11" t="n">
-        <v>3138983159</v>
+          <t>GRISELDA JOHANA PRIMERO PATERNINA</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>3223595212</t>
+        </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>3008196562</t>
+          <t>3103816400</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
@@ -1384,32 +1418,30 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>M624</t>
+          <t>Z359</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>EDGAR  EMBUZ TORRALVO</t>
-        </is>
-      </c>
-      <c r="M11" t="n">
-        <v>78</v>
-      </c>
+          <t>RAFAEL EMIRO BUELVAS LUNA</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr"/>
       <c r="N11" t="inlineStr">
         <is>
-          <t>MEDICINA GENERAL</t>
+          <t>GINECOLOGIA Y OBSTETRICIA</t>
         </is>
       </c>
       <c r="O11" t="n">
-        <v>931001</v>
+        <v>906249</v>
       </c>
       <c r="P11" t="inlineStr">
         <is>
-          <t>TERAPIA FISICA INTEGRAL SOD</t>
+          <t>VIH 1 Y 2  ANTICUERPOS PRUEBA RAPIDA</t>
         </is>
       </c>
       <c r="Q11" t="n">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="R11" t="inlineStr"/>
       <c r="S11" t="n">
@@ -1428,7 +1460,7 @@
     </row>
     <row r="12">
       <c r="A12" s="2" t="n">
-        <v>45967.57631625241</v>
+        <v>45967.79306261727</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
@@ -1451,19 +1483,21 @@
         </is>
       </c>
       <c r="F12" t="n">
-        <v>50941982</v>
+        <v>1040491654</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>NORMA DE JESUS RIVERO ARROYO</t>
-        </is>
-      </c>
-      <c r="H12" t="n">
-        <v>3137379666</v>
+          <t>GRISELDA JOHANA PRIMERO PATERNINA</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>3223595212</t>
+        </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>3145447973</t>
+          <t>3103816400</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
@@ -1473,28 +1507,26 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>K580</t>
+          <t>Z359</t>
         </is>
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>MAIRON ALDAHIR ANGULO CARVAJAL</t>
-        </is>
-      </c>
-      <c r="M12" t="n">
-        <v>78</v>
-      </c>
+          <t>RAFAEL EMIRO BUELVAS LUNA</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr"/>
       <c r="N12" t="inlineStr">
         <is>
-          <t>MEDICINA GENERAL</t>
+          <t>GINECOLOGIA Y OBSTETRICIA</t>
         </is>
       </c>
       <c r="O12" t="n">
-        <v>452301</v>
+        <v>662101</v>
       </c>
       <c r="P12" t="inlineStr">
         <is>
-          <t>COLONOSCOPIA TOTAL</t>
+          <t>ABLACION U OCLUSION DE TROMPA DE FALOPIO BILATERAL POR LAPAROTOMIA</t>
         </is>
       </c>
       <c r="Q12" t="n">
@@ -1517,7 +1549,7 @@
     </row>
     <row r="13">
       <c r="A13" s="2" t="n">
-        <v>45967.5763162533</v>
+        <v>45967.79306262882</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
@@ -1540,19 +1572,21 @@
         </is>
       </c>
       <c r="F13" t="n">
-        <v>25987708</v>
+        <v>1040491654</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>ALBA ROSA PEÑA BURGOS</t>
-        </is>
-      </c>
-      <c r="H13" t="n">
-        <v>3147707175</v>
+          <t>GRISELDA JOHANA PRIMERO PATERNINA</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>3223595212</t>
+        </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>3147707175</t>
+          <t>3103816400</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
@@ -1562,28 +1596,26 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>Z712</t>
+          <t>Z359</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>YEIDIS PATRICIA LOPEZ  BRAVO</t>
-        </is>
-      </c>
-      <c r="M13" t="n">
-        <v>78</v>
-      </c>
+          <t>RAFAEL EMIRO BUELVAS LUNA</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr"/>
       <c r="N13" t="inlineStr">
         <is>
-          <t>MEDICINA GENERAL</t>
+          <t>GINECOLOGIA Y OBSTETRICIA</t>
         </is>
       </c>
       <c r="O13" t="n">
-        <v>881332</v>
+        <v>740001</v>
       </c>
       <c r="P13" t="inlineStr">
         <is>
-          <t>ULTRASONOGRAFIA DE VÍAS URINARIAS (RIÑONES  VEJIGA Y PROSTATA TRANSABDOMINAL)</t>
+          <t>CESAREA SEGMENTARIA TRANSPERITONEAL SOD</t>
         </is>
       </c>
       <c r="Q13" t="n">
@@ -1606,7 +1638,7 @@
     </row>
     <row r="14">
       <c r="A14" s="2" t="n">
-        <v>45967.57631625411</v>
+        <v>45967.79306262882</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
@@ -1629,19 +1661,21 @@
         </is>
       </c>
       <c r="F14" t="n">
-        <v>78295035</v>
+        <v>1040491654</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>FELIX TOMAS NIÑO ROYET</t>
-        </is>
-      </c>
-      <c r="H14" t="n">
-        <v>3104540015</v>
+          <t>GRISELDA JOHANA PRIMERO PATERNINA</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>3223595212</t>
+        </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>3225042411</t>
+          <t>3103816400</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
@@ -1651,26 +1685,26 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>I10X</t>
+          <t>Z359</t>
         </is>
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>JASDANYS  SAENZ MEDRANO</t>
+          <t>RAFAEL EMIRO BUELVAS LUNA</t>
         </is>
       </c>
       <c r="M14" t="inlineStr"/>
       <c r="N14" t="inlineStr">
         <is>
-          <t>PYP MEDICO</t>
+          <t>GINECOLOGIA Y OBSTETRICIA</t>
         </is>
       </c>
       <c r="O14" t="n">
-        <v>903026</v>
+        <v>897011</v>
       </c>
       <c r="P14" t="inlineStr">
         <is>
-          <t>MICROALBUMINURIA POR EIA</t>
+          <t>MONITORIA FETAL ANTEPARTO</t>
         </is>
       </c>
       <c r="Q14" t="n">
@@ -1693,7 +1727,7 @@
     </row>
     <row r="15">
       <c r="A15" s="2" t="n">
-        <v>45967.5763162549</v>
+        <v>45967.79306262882</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
@@ -1716,19 +1750,21 @@
         </is>
       </c>
       <c r="F15" t="n">
-        <v>10970305</v>
+        <v>1063301399</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>ARGEMIRO MANUEL YANES MARMOL</t>
-        </is>
-      </c>
-      <c r="H15" t="n">
-        <v>3126870226</v>
+          <t>JOHANA DEL CARMEN MEJIA URZOLA</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>3008134457</t>
+        </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>3126870226</t>
+          <t>3143910237</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
@@ -1738,26 +1774,28 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>E119</t>
+          <t>N63X</t>
         </is>
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>JASDANYS  SAENZ MEDRANO</t>
-        </is>
-      </c>
-      <c r="M15" t="inlineStr"/>
+          <t>DANIELA ALEXANDRA PEREZ CORDERO</t>
+        </is>
+      </c>
+      <c r="M15" t="n">
+        <v>78</v>
+      </c>
       <c r="N15" t="inlineStr">
         <is>
-          <t>PYP MEDICO</t>
+          <t>MEDICINA GENERAL</t>
         </is>
       </c>
       <c r="O15" t="n">
-        <v>903026</v>
+        <v>904108</v>
       </c>
       <c r="P15" t="inlineStr">
         <is>
-          <t>MICROALBUMINURIA POR EIA</t>
+          <t>PROLACTINA BASAL</t>
         </is>
       </c>
       <c r="Q15" t="n">
@@ -1780,7 +1818,7 @@
     </row>
     <row r="16">
       <c r="A16" s="2" t="n">
-        <v>45967.57631625568</v>
+        <v>45967.79306262882</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
@@ -1799,23 +1837,25 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>TI</t>
+          <t>CC</t>
         </is>
       </c>
       <c r="F16" t="n">
-        <v>1063303459</v>
+        <v>1063301399</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>DULCE PAZ ARRIETA FLOREZ</t>
-        </is>
-      </c>
-      <c r="H16" t="n">
-        <v>3107944215</v>
+          <t>JOHANA DEL CARMEN MEJIA URZOLA</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>3008134457</t>
+        </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>3107944215</t>
+          <t>3143910237</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
@@ -1825,26 +1865,28 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>Z002</t>
+          <t>N63X</t>
         </is>
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>PAULA ANDREA AGUAS VERGARA</t>
-        </is>
-      </c>
-      <c r="M16" t="inlineStr"/>
+          <t>DANIELA ALEXANDRA PEREZ CORDERO</t>
+        </is>
+      </c>
+      <c r="M16" t="n">
+        <v>78</v>
+      </c>
       <c r="N16" t="inlineStr">
         <is>
-          <t>PYP ENFERMERIA</t>
+          <t>MEDICINA GENERAL</t>
         </is>
       </c>
       <c r="O16" t="n">
-        <v>194140</v>
+        <v>906039</v>
       </c>
       <c r="P16" t="inlineStr">
         <is>
-          <t>MÉDICO U ODONTÓLOGO GENERAL</t>
+          <t>TREPONEMA PALLIDUM  - Prueba Rapida</t>
         </is>
       </c>
       <c r="Q16" t="n">
@@ -1867,7 +1909,7 @@
     </row>
     <row r="17">
       <c r="A17" s="2" t="n">
-        <v>45967.57631625645</v>
+        <v>45967.79306264036</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
@@ -1890,19 +1932,21 @@
         </is>
       </c>
       <c r="F17" t="n">
-        <v>1040491654</v>
+        <v>1063301399</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>GRISELDA JOHANA PRIMERO PATERNINA</t>
-        </is>
-      </c>
-      <c r="H17" t="n">
-        <v>3223595212</v>
+          <t>JOHANA DEL CARMEN MEJIA URZOLA</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>3008134457</t>
+        </is>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>3103816400</t>
+          <t>3143910237</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
@@ -1912,18 +1956,20 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>Z359</t>
+          <t>N63X</t>
         </is>
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>RAFAEL EMIRO BUELVAS LUNA</t>
-        </is>
-      </c>
-      <c r="M17" t="inlineStr"/>
+          <t>DANIELA ALEXANDRA PEREZ CORDERO</t>
+        </is>
+      </c>
+      <c r="M17" t="n">
+        <v>78</v>
+      </c>
       <c r="N17" t="inlineStr">
         <is>
-          <t>GINECOLOGIA Y OBSTETRICIA</t>
+          <t>MEDICINA GENERAL</t>
         </is>
       </c>
       <c r="O17" t="n">
@@ -1954,7 +2000,7 @@
     </row>
     <row r="18">
       <c r="A18" s="2" t="n">
-        <v>45967.57631625721</v>
+        <v>45967.79306264036</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
@@ -1977,19 +2023,21 @@
         </is>
       </c>
       <c r="F18" t="n">
-        <v>1040491654</v>
+        <v>1063301399</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>GRISELDA JOHANA PRIMERO PATERNINA</t>
-        </is>
-      </c>
-      <c r="H18" t="n">
-        <v>3223595212</v>
+          <t>JOHANA DEL CARMEN MEJIA URZOLA</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>3008134457</t>
+        </is>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>3103816400</t>
+          <t>3143910237</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
@@ -1999,26 +2047,28 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>Z359</t>
+          <t>N63X</t>
         </is>
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>RAFAEL EMIRO BUELVAS LUNA</t>
-        </is>
-      </c>
-      <c r="M18" t="inlineStr"/>
+          <t>DANIELA ALEXANDRA PEREZ CORDERO</t>
+        </is>
+      </c>
+      <c r="M18" t="n">
+        <v>78</v>
+      </c>
       <c r="N18" t="inlineStr">
         <is>
-          <t>GINECOLOGIA Y OBSTETRICIA</t>
+          <t>MEDICINA GENERAL</t>
         </is>
       </c>
       <c r="O18" t="n">
-        <v>662101</v>
+        <v>881201</v>
       </c>
       <c r="P18" t="inlineStr">
         <is>
-          <t>ABLACION U OCLUSION DE TROMPA DE FALOPIO BILATERAL POR LAPAROTOMIA</t>
+          <t>ULTRASONOGRAFIA DIAGNOSTICA DE MAMA  CON TRANSDUCTOR DE 7 MHZ O MAS</t>
         </is>
       </c>
       <c r="Q18" t="n">
@@ -2041,7 +2091,7 @@
     </row>
     <row r="19">
       <c r="A19" s="2" t="n">
-        <v>45967.57631625798</v>
+        <v>45967.79306264036</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
@@ -2064,21 +2114,15 @@
         </is>
       </c>
       <c r="F19" t="n">
-        <v>1040491654</v>
+        <v>17076612</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>GRISELDA JOHANA PRIMERO PATERNINA</t>
-        </is>
-      </c>
-      <c r="H19" t="n">
-        <v>3223595212</v>
-      </c>
-      <c r="I19" t="inlineStr">
-        <is>
-          <t>3103816400</t>
-        </is>
-      </c>
+          <t>CARLOS  CRUZ SERNA</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr"/>
+      <c r="I19" t="inlineStr"/>
       <c r="J19" t="inlineStr">
         <is>
           <t>05/11/2025</t>
@@ -2086,26 +2130,28 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>Z359</t>
+          <t>E119</t>
         </is>
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>RAFAEL EMIRO BUELVAS LUNA</t>
-        </is>
-      </c>
-      <c r="M19" t="inlineStr"/>
+          <t>MAIRON ALDAHIR ANGULO CARVAJAL</t>
+        </is>
+      </c>
+      <c r="M19" t="n">
+        <v>78</v>
+      </c>
       <c r="N19" t="inlineStr">
         <is>
-          <t>GINECOLOGIA Y OBSTETRICIA</t>
+          <t>MEDICINA GENERAL</t>
         </is>
       </c>
       <c r="O19" t="n">
-        <v>740001</v>
+        <v>903844</v>
       </c>
       <c r="P19" t="inlineStr">
         <is>
-          <t>CESAREA SEGMENTARIA TRANSPERITONEAL SOD</t>
+          <t>GLUCOSA  CURVA DE TOLERANCIA</t>
         </is>
       </c>
       <c r="Q19" t="n">
@@ -2128,7 +2174,7 @@
     </row>
     <row r="20">
       <c r="A20" s="2" t="n">
-        <v>45967.57631625875</v>
+        <v>45967.79306264036</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
@@ -2151,19 +2197,21 @@
         </is>
       </c>
       <c r="F20" t="n">
-        <v>1040491654</v>
+        <v>1148438567</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>GRISELDA JOHANA PRIMERO PATERNINA</t>
-        </is>
-      </c>
-      <c r="H20" t="n">
-        <v>3223595212</v>
+          <t>LUIS EDUARDO CALDERA HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>3245891408</t>
+        </is>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>3103816400</t>
+          <t>3022552259</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
@@ -2173,26 +2221,28 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>Z359</t>
+          <t>K769</t>
         </is>
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>RAFAEL EMIRO BUELVAS LUNA</t>
-        </is>
-      </c>
-      <c r="M20" t="inlineStr"/>
+          <t>DANIELA ALEXANDRA PEREZ CORDERO</t>
+        </is>
+      </c>
+      <c r="M20" t="n">
+        <v>78</v>
+      </c>
       <c r="N20" t="inlineStr">
         <is>
-          <t>GINECOLOGIA Y OBSTETRICIA</t>
+          <t>MEDICINA GENERAL</t>
         </is>
       </c>
       <c r="O20" t="n">
-        <v>897011</v>
+        <v>903043</v>
       </c>
       <c r="P20" t="inlineStr">
         <is>
-          <t>MONITORIA FETAL ANTEPARTO</t>
+          <t>PRUEBA DE ALIENTO 13 C UREA PARA HELICOBACTER PILORY</t>
         </is>
       </c>
       <c r="Q20" t="n">
@@ -2215,7 +2265,7 @@
     </row>
     <row r="21">
       <c r="A21" s="2" t="n">
-        <v>45967.57631625951</v>
+        <v>45967.79306264036</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
@@ -2234,21 +2284,25 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>TI</t>
+          <t>CC</t>
         </is>
       </c>
       <c r="F21" t="n">
-        <v>1063298147</v>
+        <v>1148438567</v>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>SARA LUCIA TIRADO HERNANDEZ</t>
-        </is>
-      </c>
-      <c r="H21" t="inlineStr"/>
+          <t>LUIS EDUARDO CALDERA HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>3245891408</t>
+        </is>
+      </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>3215236383</t>
+          <t>3022552259</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
@@ -2258,26 +2312,28 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>Z003</t>
+          <t>K769</t>
         </is>
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>KAREN GISELLE CARRILLO NAVARRO</t>
-        </is>
-      </c>
-      <c r="M21" t="inlineStr"/>
+          <t>DANIELA ALEXANDRA PEREZ CORDERO</t>
+        </is>
+      </c>
+      <c r="M21" t="n">
+        <v>78</v>
+      </c>
       <c r="N21" t="inlineStr">
         <is>
-          <t>PYP ENFERMERIA</t>
+          <t>MEDICINA GENERAL</t>
         </is>
       </c>
       <c r="O21" t="n">
-        <v>890207</v>
+        <v>903809</v>
       </c>
       <c r="P21" t="inlineStr">
         <is>
-          <t>CONSULTA DE PRIMERA VEZ POR OPTOMETRIA</t>
+          <t>BILIRRUBINAS TOTAL Y DIRECTA</t>
         </is>
       </c>
       <c r="Q21" t="n">
@@ -2300,7 +2356,7 @@
     </row>
     <row r="22">
       <c r="A22" s="2" t="n">
-        <v>45967.57631626027</v>
+        <v>45967.79306264036</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
@@ -2323,19 +2379,21 @@
         </is>
       </c>
       <c r="F22" t="n">
-        <v>1063301399</v>
+        <v>1148438567</v>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>JOHANA DEL CARMEN MEJIA URZOLA</t>
-        </is>
-      </c>
-      <c r="H22" t="n">
-        <v>3008134457</v>
+          <t>LUIS EDUARDO CALDERA HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>3245891408</t>
+        </is>
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>3143910237</t>
+          <t>3022552259</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
@@ -2345,7 +2403,7 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>N63X</t>
+          <t>K769</t>
         </is>
       </c>
       <c r="L22" t="inlineStr">
@@ -2362,11 +2420,11 @@
         </is>
       </c>
       <c r="O22" t="n">
-        <v>904108</v>
+        <v>903866</v>
       </c>
       <c r="P22" t="inlineStr">
         <is>
-          <t>PROLACTINA BASAL</t>
+          <t>TRANSAMINASA GLUTÁMICOPIRÚVICA O ALANINO AMINO TRANSFE-RASA TGP-ALT *</t>
         </is>
       </c>
       <c r="Q22" t="n">
@@ -2389,7 +2447,7 @@
     </row>
     <row r="23">
       <c r="A23" s="2" t="n">
-        <v>45967.57631626104</v>
+        <v>45967.79306264036</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
@@ -2412,19 +2470,21 @@
         </is>
       </c>
       <c r="F23" t="n">
-        <v>1063301399</v>
+        <v>1148438567</v>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>JOHANA DEL CARMEN MEJIA URZOLA</t>
-        </is>
-      </c>
-      <c r="H23" t="n">
-        <v>3008134457</v>
+          <t>LUIS EDUARDO CALDERA HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>3245891408</t>
+        </is>
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>3143910237</t>
+          <t>3022552259</t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
@@ -2434,7 +2494,7 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>N63X</t>
+          <t>K769</t>
         </is>
       </c>
       <c r="L23" t="inlineStr">
@@ -2451,11 +2511,11 @@
         </is>
       </c>
       <c r="O23" t="n">
-        <v>906039</v>
+        <v>903867</v>
       </c>
       <c r="P23" t="inlineStr">
         <is>
-          <t>TREPONEMA PALLIDUM  - Prueba Rapida</t>
+          <t>TRANSAMINASA GLUTÁMICO OXALACÉTICA O ASPARTATO AMINO TRANSFERASA TGO-AST</t>
         </is>
       </c>
       <c r="Q23" t="n">
@@ -2478,7 +2538,7 @@
     </row>
     <row r="24">
       <c r="A24" s="2" t="n">
-        <v>45967.5763162618</v>
+        <v>45967.793062652</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
@@ -2501,19 +2561,21 @@
         </is>
       </c>
       <c r="F24" t="n">
-        <v>1063301399</v>
+        <v>1066744542</v>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>JOHANA DEL CARMEN MEJIA URZOLA</t>
-        </is>
-      </c>
-      <c r="H24" t="n">
-        <v>3008134457</v>
+          <t>KATHERINE  OTERO FURNIELES</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>3114221804</t>
+        </is>
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>3143910237</t>
+          <t>3114551804</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
@@ -2523,28 +2585,26 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>N63X</t>
+          <t>Z359</t>
         </is>
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>DANIELA ALEXANDRA PEREZ CORDERO</t>
-        </is>
-      </c>
-      <c r="M24" t="n">
-        <v>78</v>
-      </c>
+          <t>RAFAEL EMIRO BUELVAS LUNA</t>
+        </is>
+      </c>
+      <c r="M24" t="inlineStr"/>
       <c r="N24" t="inlineStr">
         <is>
-          <t>MEDICINA GENERAL</t>
+          <t>GINECOLOGIA Y OBSTETRICIA</t>
         </is>
       </c>
       <c r="O24" t="n">
-        <v>906249</v>
+        <v>897011</v>
       </c>
       <c r="P24" t="inlineStr">
         <is>
-          <t>VIH 1 Y 2  ANTICUERPOS PRUEBA RAPIDA</t>
+          <t>MONITORIA FETAL ANTEPARTO</t>
         </is>
       </c>
       <c r="Q24" t="n">
@@ -2567,7 +2627,7 @@
     </row>
     <row r="25">
       <c r="A25" s="2" t="n">
-        <v>45967.57631626257</v>
+        <v>45967.793062652</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
@@ -2590,21 +2650,19 @@
         </is>
       </c>
       <c r="F25" t="n">
-        <v>1063301399</v>
+        <v>78304433</v>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>JOHANA DEL CARMEN MEJIA URZOLA</t>
-        </is>
-      </c>
-      <c r="H25" t="n">
-        <v>3008134457</v>
-      </c>
-      <c r="I25" t="inlineStr">
-        <is>
-          <t>3143910237</t>
-        </is>
-      </c>
+          <t>ADRIAN DE JESUS CASTAÑO HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>3126873291</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr"/>
       <c r="J25" t="inlineStr">
         <is>
           <t>05/11/2025</t>
@@ -2612,12 +2670,12 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>N63X</t>
+          <t>Z008</t>
         </is>
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>DANIELA ALEXANDRA PEREZ CORDERO</t>
+          <t>EDGAR  ACOSTA GANDIA</t>
         </is>
       </c>
       <c r="M25" t="n">
@@ -2629,20 +2687,18 @@
         </is>
       </c>
       <c r="O25" t="n">
-        <v>881201</v>
+        <v>906610</v>
       </c>
       <c r="P25" t="inlineStr">
         <is>
-          <t>ULTRASONOGRAFIA DIAGNOSTICA DE MAMA  CON TRANSDUCTOR DE 7 MHZ O MAS</t>
+          <t>ANTIGENO ESPECIFICO DE PROSTATA PSA</t>
         </is>
       </c>
       <c r="Q25" t="n">
         <v>1</v>
       </c>
       <c r="R25" t="inlineStr"/>
-      <c r="S25" t="n">
-        <v>0</v>
-      </c>
+      <c r="S25" t="inlineStr"/>
       <c r="T25" t="inlineStr"/>
       <c r="U25" t="inlineStr"/>
       <c r="V25" t="inlineStr"/>
@@ -2656,7 +2712,7 @@
     </row>
     <row r="26">
       <c r="A26" s="2" t="n">
-        <v>45967.57631626354</v>
+        <v>45967.793062652</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
@@ -2679,14 +2735,18 @@
         </is>
       </c>
       <c r="F26" t="n">
-        <v>17076612</v>
+        <v>78304433</v>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>CARLOS  CRUZ SERNA</t>
-        </is>
-      </c>
-      <c r="H26" t="inlineStr"/>
+          <t>ADRIAN DE JESUS CASTAÑO HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>3126873291</t>
+        </is>
+      </c>
       <c r="I26" t="inlineStr"/>
       <c r="J26" t="inlineStr">
         <is>
@@ -2695,12 +2755,12 @@
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>E119</t>
+          <t>Z008</t>
         </is>
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>MAIRON ALDAHIR ANGULO CARVAJAL</t>
+          <t>EDGAR  ACOSTA GANDIA</t>
         </is>
       </c>
       <c r="M26" t="n">
@@ -2712,20 +2772,18 @@
         </is>
       </c>
       <c r="O26" t="n">
-        <v>903844</v>
+        <v>881502</v>
       </c>
       <c r="P26" t="inlineStr">
         <is>
-          <t>GLUCOSA  CURVA DE TOLERANCIA</t>
+          <t>ULTRASONOGRAFÍA DE PROSTATA TRANSRECTAL</t>
         </is>
       </c>
       <c r="Q26" t="n">
         <v>1</v>
       </c>
       <c r="R26" t="inlineStr"/>
-      <c r="S26" t="n">
-        <v>0</v>
-      </c>
+      <c r="S26" t="inlineStr"/>
       <c r="T26" t="inlineStr"/>
       <c r="U26" t="inlineStr"/>
       <c r="V26" t="inlineStr"/>
@@ -2739,7 +2797,7 @@
     </row>
     <row r="27">
       <c r="A27" s="2" t="n">
-        <v>45967.5763162644</v>
+        <v>45967.793062652</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
@@ -2762,19 +2820,21 @@
         </is>
       </c>
       <c r="F27" t="n">
-        <v>1148438567</v>
+        <v>50998478</v>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>LUIS EDUARDO CALDERA HERNANDEZ</t>
-        </is>
-      </c>
-      <c r="H27" t="n">
-        <v>3245891408</v>
+          <t>DORCA YANETH JARAMILLO RAMOS</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>3103973448</t>
+        </is>
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>3022552259</t>
+          <t>3103973448</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
@@ -2784,12 +2844,12 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>K769</t>
+          <t>Z008</t>
         </is>
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>DANIELA ALEXANDRA PEREZ CORDERO</t>
+          <t>CAMILA JOHANA PACITO DIAZ</t>
         </is>
       </c>
       <c r="M27" t="n">
@@ -2801,11 +2861,11 @@
         </is>
       </c>
       <c r="O27" t="n">
-        <v>903043</v>
+        <v>904902</v>
       </c>
       <c r="P27" t="inlineStr">
         <is>
-          <t>PRUEBA DE ALIENTO 13 C UREA PARA HELICOBACTER PILORY</t>
+          <t>HORMONA ESTIMULANTE DEL TIROIDES TSH</t>
         </is>
       </c>
       <c r="Q27" t="n">
@@ -2828,7 +2888,7 @@
     </row>
     <row r="28">
       <c r="A28" s="2" t="n">
-        <v>45967.57631626521</v>
+        <v>45967.793062652</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
@@ -2851,19 +2911,21 @@
         </is>
       </c>
       <c r="F28" t="n">
-        <v>1148438567</v>
+        <v>50998478</v>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>LUIS EDUARDO CALDERA HERNANDEZ</t>
-        </is>
-      </c>
-      <c r="H28" t="n">
-        <v>3245891408</v>
+          <t>DORCA YANETH JARAMILLO RAMOS</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>3103973448</t>
+        </is>
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>3022552259</t>
+          <t>3103973448</t>
         </is>
       </c>
       <c r="J28" t="inlineStr">
@@ -2873,12 +2935,12 @@
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>K769</t>
+          <t>Z008</t>
         </is>
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>DANIELA ALEXANDRA PEREZ CORDERO</t>
+          <t>CAMILA JOHANA PACITO DIAZ</t>
         </is>
       </c>
       <c r="M28" t="n">
@@ -2890,11 +2952,11 @@
         </is>
       </c>
       <c r="O28" t="n">
-        <v>903809</v>
+        <v>904921</v>
       </c>
       <c r="P28" t="inlineStr">
         <is>
-          <t>BILIRRUBINAS TOTAL Y DIRECTA</t>
+          <t>TIROXINA LIBRE T4L</t>
         </is>
       </c>
       <c r="Q28" t="n">
@@ -2917,7 +2979,7 @@
     </row>
     <row r="29">
       <c r="A29" s="2" t="n">
-        <v>45967.57631626597</v>
+        <v>45967.793062652</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
@@ -2940,19 +3002,21 @@
         </is>
       </c>
       <c r="F29" t="n">
-        <v>1148438567</v>
+        <v>50998478</v>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>LUIS EDUARDO CALDERA HERNANDEZ</t>
-        </is>
-      </c>
-      <c r="H29" t="n">
-        <v>3245891408</v>
+          <t>DORCA YANETH JARAMILLO RAMOS</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>3103973448</t>
+        </is>
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>3022552259</t>
+          <t>3103973448</t>
         </is>
       </c>
       <c r="J29" t="inlineStr">
@@ -2962,12 +3026,12 @@
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>K769</t>
+          <t>Z008</t>
         </is>
       </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>DANIELA ALEXANDRA PEREZ CORDERO</t>
+          <t>CAMILA JOHANA PACITO DIAZ</t>
         </is>
       </c>
       <c r="M29" t="n">
@@ -2979,11 +3043,11 @@
         </is>
       </c>
       <c r="O29" t="n">
-        <v>903866</v>
+        <v>904924</v>
       </c>
       <c r="P29" t="inlineStr">
         <is>
-          <t>TRANSAMINASA GLUTÁMICOPIRÚVICA O ALANINO AMINO TRANSFE-RASA TGP-ALT *</t>
+          <t>TRIYODOTIRONINA LIBRE T3L</t>
         </is>
       </c>
       <c r="Q29" t="n">
@@ -3006,7 +3070,7 @@
     </row>
     <row r="30">
       <c r="A30" s="2" t="n">
-        <v>45967.57631626674</v>
+        <v>45967.79306266351</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
@@ -3025,25 +3089,19 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>CC</t>
+          <t>TI</t>
         </is>
       </c>
       <c r="F30" t="n">
-        <v>1148438567</v>
+        <v>1063301201</v>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>LUIS EDUARDO CALDERA HERNANDEZ</t>
-        </is>
-      </c>
-      <c r="H30" t="n">
-        <v>3245891408</v>
-      </c>
-      <c r="I30" t="inlineStr">
-        <is>
-          <t>3022552259</t>
-        </is>
-      </c>
+          <t>SHAIRA SAMIR MENDOZA MENESES</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr"/>
+      <c r="I30" t="inlineStr"/>
       <c r="J30" t="inlineStr">
         <is>
           <t>05/11/2025</t>
@@ -3051,12 +3109,12 @@
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>K769</t>
+          <t>R509</t>
         </is>
       </c>
       <c r="L30" t="inlineStr">
         <is>
-          <t>DANIELA ALEXANDRA PEREZ CORDERO</t>
+          <t>SANTIAGO  AGUDELO VILORIA</t>
         </is>
       </c>
       <c r="M30" t="n">
@@ -3068,11 +3126,11 @@
         </is>
       </c>
       <c r="O30" t="n">
-        <v>903867</v>
+        <v>902204</v>
       </c>
       <c r="P30" t="inlineStr">
         <is>
-          <t>TRANSAMINASA GLUTÁMICO OXALACÉTICA O ASPARTATO AMINO TRANSFERASA TGO-AST</t>
+          <t>ERITROSEDIMENTACION VELOCIDAD SEDIMENTACION GLOBULAR - VSG</t>
         </is>
       </c>
       <c r="Q30" t="n">
@@ -3095,7 +3153,7 @@
     </row>
     <row r="31">
       <c r="A31" s="2" t="n">
-        <v>45967.57631626748</v>
+        <v>45967.79306266351</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
@@ -3114,25 +3172,19 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>CC</t>
+          <t>TI</t>
         </is>
       </c>
       <c r="F31" t="n">
-        <v>1066744542</v>
+        <v>1063301201</v>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>KATHERINE  OTERO FURNIELES</t>
-        </is>
-      </c>
-      <c r="H31" t="n">
-        <v>3114221804</v>
-      </c>
-      <c r="I31" t="inlineStr">
-        <is>
-          <t>3114551804</t>
-        </is>
-      </c>
+          <t>SHAIRA SAMIR MENDOZA MENESES</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr"/>
+      <c r="I31" t="inlineStr"/>
       <c r="J31" t="inlineStr">
         <is>
           <t>05/11/2025</t>
@@ -3140,26 +3192,28 @@
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>Z359</t>
+          <t>R509</t>
         </is>
       </c>
       <c r="L31" t="inlineStr">
         <is>
-          <t>RAFAEL EMIRO BUELVAS LUNA</t>
-        </is>
-      </c>
-      <c r="M31" t="inlineStr"/>
+          <t>SANTIAGO  AGUDELO VILORIA</t>
+        </is>
+      </c>
+      <c r="M31" t="n">
+        <v>78</v>
+      </c>
       <c r="N31" t="inlineStr">
         <is>
-          <t>GINECOLOGIA Y OBSTETRICIA</t>
+          <t>MEDICINA GENERAL</t>
         </is>
       </c>
       <c r="O31" t="n">
-        <v>897011</v>
+        <v>906208</v>
       </c>
       <c r="P31" t="inlineStr">
         <is>
-          <t>MONITORIA FETAL ANTEPARTO</t>
+          <t>DENGUE  ANTICUERPOS IG M</t>
         </is>
       </c>
       <c r="Q31" t="n">
@@ -3182,7 +3236,7 @@
     </row>
     <row r="32">
       <c r="A32" s="2" t="n">
-        <v>45967.57631626824</v>
+        <v>45967.79306266351</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
@@ -3205,17 +3259,23 @@
         </is>
       </c>
       <c r="F32" t="n">
-        <v>78304433</v>
+        <v>1003337179</v>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>ADRIAN DE JESUS CASTAÑO HERNANDEZ</t>
-        </is>
-      </c>
-      <c r="H32" t="n">
-        <v>3126873291</v>
-      </c>
-      <c r="I32" t="inlineStr"/>
+          <t>CARMEN   SEÑA GUERRA</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>3103963600</t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>3106765113</t>
+        </is>
+      </c>
       <c r="J32" t="inlineStr">
         <is>
           <t>05/11/2025</t>
@@ -3223,12 +3283,12 @@
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>Z008</t>
+          <t>R074</t>
         </is>
       </c>
       <c r="L32" t="inlineStr">
         <is>
-          <t>EDGAR  ACOSTA GANDIA</t>
+          <t>DANIELA ALEXANDRA PEREZ CORDERO</t>
         </is>
       </c>
       <c r="M32" t="n">
@@ -3240,18 +3300,20 @@
         </is>
       </c>
       <c r="O32" t="n">
-        <v>906610</v>
+        <v>906039</v>
       </c>
       <c r="P32" t="inlineStr">
         <is>
-          <t>ANTIGENO ESPECIFICO DE PROSTATA PSA</t>
+          <t>TREPONEMA PALLIDUM  - Prueba Rapida</t>
         </is>
       </c>
       <c r="Q32" t="n">
         <v>1</v>
       </c>
       <c r="R32" t="inlineStr"/>
-      <c r="S32" t="inlineStr"/>
+      <c r="S32" t="n">
+        <v>0</v>
+      </c>
       <c r="T32" t="inlineStr"/>
       <c r="U32" t="inlineStr"/>
       <c r="V32" t="inlineStr"/>
@@ -3265,7 +3327,7 @@
     </row>
     <row r="33">
       <c r="A33" s="2" t="n">
-        <v>45967.57631626901</v>
+        <v>45967.79306266351</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
@@ -3288,17 +3350,23 @@
         </is>
       </c>
       <c r="F33" t="n">
-        <v>78304433</v>
+        <v>1003337179</v>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>ADRIAN DE JESUS CASTAÑO HERNANDEZ</t>
-        </is>
-      </c>
-      <c r="H33" t="n">
-        <v>3126873291</v>
-      </c>
-      <c r="I33" t="inlineStr"/>
+          <t>CARMEN   SEÑA GUERRA</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>3103963600</t>
+        </is>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>3106765113</t>
+        </is>
+      </c>
       <c r="J33" t="inlineStr">
         <is>
           <t>05/11/2025</t>
@@ -3306,12 +3374,12 @@
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>Z008</t>
+          <t>R074</t>
         </is>
       </c>
       <c r="L33" t="inlineStr">
         <is>
-          <t>EDGAR  ACOSTA GANDIA</t>
+          <t>DANIELA ALEXANDRA PEREZ CORDERO</t>
         </is>
       </c>
       <c r="M33" t="n">
@@ -3323,18 +3391,20 @@
         </is>
       </c>
       <c r="O33" t="n">
-        <v>881502</v>
+        <v>906249</v>
       </c>
       <c r="P33" t="inlineStr">
         <is>
-          <t>ULTRASONOGRAFÍA DE PROSTATA TRANSRECTAL</t>
+          <t>VIH 1 Y 2  ANTICUERPOS PRUEBA RAPIDA</t>
         </is>
       </c>
       <c r="Q33" t="n">
         <v>1</v>
       </c>
       <c r="R33" t="inlineStr"/>
-      <c r="S33" t="inlineStr"/>
+      <c r="S33" t="n">
+        <v>0</v>
+      </c>
       <c r="T33" t="inlineStr"/>
       <c r="U33" t="inlineStr"/>
       <c r="V33" t="inlineStr"/>
@@ -3348,7 +3418,7 @@
     </row>
     <row r="34">
       <c r="A34" s="2" t="n">
-        <v>45967.57631626977</v>
+        <v>45967.79306266351</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
@@ -3371,19 +3441,21 @@
         </is>
       </c>
       <c r="F34" t="n">
-        <v>10994395</v>
+        <v>22533915</v>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>ANDRES ANTONIO PEREZ BANQUET</t>
-        </is>
-      </c>
-      <c r="H34" t="n">
-        <v>3245638022</v>
+          <t>LEANA PATRICIA MUÑOZ JIMENEZ</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>3216702029</t>
+        </is>
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>3106077702</t>
+          <t>3156606596</t>
         </is>
       </c>
       <c r="J34" t="inlineStr">
@@ -3393,26 +3465,28 @@
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>N189</t>
+          <t>R074</t>
         </is>
       </c>
       <c r="L34" t="inlineStr">
         <is>
-          <t>JASDANYS  SAENZ MEDRANO</t>
-        </is>
-      </c>
-      <c r="M34" t="inlineStr"/>
+          <t>DANIELA ALEXANDRA PEREZ CORDERO</t>
+        </is>
+      </c>
+      <c r="M34" t="n">
+        <v>78</v>
+      </c>
       <c r="N34" t="inlineStr">
         <is>
-          <t>PYP MEDICO</t>
+          <t>MEDICINA GENERAL</t>
         </is>
       </c>
       <c r="O34" t="n">
-        <v>903026</v>
+        <v>903801</v>
       </c>
       <c r="P34" t="inlineStr">
         <is>
-          <t>MICROALBUMINURIA POR EIA</t>
+          <t>ACIDO URICO O:P</t>
         </is>
       </c>
       <c r="Q34" t="n">
@@ -3435,7 +3509,7 @@
     </row>
     <row r="35">
       <c r="A35" s="2" t="n">
-        <v>45967.57631627054</v>
+        <v>45967.79306266351</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
@@ -3458,19 +3532,21 @@
         </is>
       </c>
       <c r="F35" t="n">
-        <v>50998478</v>
+        <v>22533915</v>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>DORCA YANETH JARAMILLO RAMOS</t>
-        </is>
-      </c>
-      <c r="H35" t="n">
-        <v>3103973448</v>
+          <t>LEANA PATRICIA MUÑOZ JIMENEZ</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>3216702029</t>
+        </is>
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>3103973448</t>
+          <t>3156606596</t>
         </is>
       </c>
       <c r="J35" t="inlineStr">
@@ -3480,12 +3556,12 @@
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>Z008</t>
+          <t>R074</t>
         </is>
       </c>
       <c r="L35" t="inlineStr">
         <is>
-          <t>CAMILA JOHANA PACITO DIAZ</t>
+          <t>DANIELA ALEXANDRA PEREZ CORDERO</t>
         </is>
       </c>
       <c r="M35" t="n">
@@ -3497,11 +3573,11 @@
         </is>
       </c>
       <c r="O35" t="n">
-        <v>904902</v>
+        <v>906914</v>
       </c>
       <c r="P35" t="inlineStr">
         <is>
-          <t>HORMONA ESTIMULANTE DEL TIROIDES TSH</t>
+          <t>PROTEÍNA C REACTIVA  PRUEBA SEMICUANTITATIVA</t>
         </is>
       </c>
       <c r="Q35" t="n">
@@ -3524,7 +3600,7 @@
     </row>
     <row r="36">
       <c r="A36" s="2" t="n">
-        <v>45967.5763162713</v>
+        <v>45967.79306266351</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
@@ -3547,19 +3623,21 @@
         </is>
       </c>
       <c r="F36" t="n">
-        <v>50998478</v>
+        <v>22533915</v>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>DORCA YANETH JARAMILLO RAMOS</t>
-        </is>
-      </c>
-      <c r="H36" t="n">
-        <v>3103973448</v>
+          <t>LEANA PATRICIA MUÑOZ JIMENEZ</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>3216702029</t>
+        </is>
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>3103973448</t>
+          <t>3156606596</t>
         </is>
       </c>
       <c r="J36" t="inlineStr">
@@ -3569,12 +3647,12 @@
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>Z008</t>
+          <t>R074</t>
         </is>
       </c>
       <c r="L36" t="inlineStr">
         <is>
-          <t>CAMILA JOHANA PACITO DIAZ</t>
+          <t>DANIELA ALEXANDRA PEREZ CORDERO</t>
         </is>
       </c>
       <c r="M36" t="n">
@@ -3586,11 +3664,11 @@
         </is>
       </c>
       <c r="O36" t="n">
-        <v>904921</v>
+        <v>906914</v>
       </c>
       <c r="P36" t="inlineStr">
         <is>
-          <t>TIROXINA LIBRE T4L</t>
+          <t>PROTEÍNA C REACTIVA  PRUEBA SEMICUANTITATIVA</t>
         </is>
       </c>
       <c r="Q36" t="n">
@@ -3613,7 +3691,7 @@
     </row>
     <row r="37">
       <c r="A37" s="2" t="n">
-        <v>45967.57631627206</v>
+        <v>45967.79306266351</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
@@ -3636,19 +3714,21 @@
         </is>
       </c>
       <c r="F37" t="n">
-        <v>50998478</v>
+        <v>1017148528</v>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>DORCA YANETH JARAMILLO RAMOS</t>
-        </is>
-      </c>
-      <c r="H37" t="n">
-        <v>3103973448</v>
+          <t>TANIA ROSA ARGUMEDO MADERA</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>3106303540</t>
+        </is>
       </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t>3103973448</t>
+          <t>3116800494</t>
         </is>
       </c>
       <c r="J37" t="inlineStr">
@@ -3663,7 +3743,7 @@
       </c>
       <c r="L37" t="inlineStr">
         <is>
-          <t>CAMILA JOHANA PACITO DIAZ</t>
+          <t>EDGAR  ACOSTA GANDIA</t>
         </is>
       </c>
       <c r="M37" t="n">
@@ -3675,20 +3755,18 @@
         </is>
       </c>
       <c r="O37" t="n">
-        <v>904924</v>
+        <v>903801</v>
       </c>
       <c r="P37" t="inlineStr">
         <is>
-          <t>TRIYODOTIRONINA LIBRE T3L</t>
+          <t>ACIDO URICO O:P</t>
         </is>
       </c>
       <c r="Q37" t="n">
         <v>1</v>
       </c>
       <c r="R37" t="inlineStr"/>
-      <c r="S37" t="n">
-        <v>0</v>
-      </c>
+      <c r="S37" t="inlineStr"/>
       <c r="T37" t="inlineStr"/>
       <c r="U37" t="inlineStr"/>
       <c r="V37" t="inlineStr"/>
@@ -3702,7 +3780,7 @@
     </row>
     <row r="38">
       <c r="A38" s="2" t="n">
-        <v>45967.57631627281</v>
+        <v>45967.79306267514</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
@@ -3725,15 +3803,23 @@
         </is>
       </c>
       <c r="F38" t="n">
-        <v>1063301201</v>
+        <v>1066605496</v>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>SHAIRA SAMIR MENDOZA MENESES</t>
-        </is>
-      </c>
-      <c r="H38" t="inlineStr"/>
-      <c r="I38" t="inlineStr"/>
+          <t>WILLIAM JOSE PADRON MONTES</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>3006352654</t>
+        </is>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>3008161877</t>
+        </is>
+      </c>
       <c r="J38" t="inlineStr">
         <is>
           <t>05/11/2025</t>
@@ -3741,12 +3827,12 @@
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>R509</t>
+          <t>S411</t>
         </is>
       </c>
       <c r="L38" t="inlineStr">
         <is>
-          <t>SANTIAGO  AGUDELO VILORIA</t>
+          <t>PAOLA CRISTINA HERAZO MIRANDA</t>
         </is>
       </c>
       <c r="M38" t="n">
@@ -3758,11 +3844,11 @@
         </is>
       </c>
       <c r="O38" t="n">
-        <v>902204</v>
+        <v>865101</v>
       </c>
       <c r="P38" t="inlineStr">
         <is>
-          <t>ERITROSEDIMENTACION VELOCIDAD SEDIMENTACION GLOBULAR - VSG</t>
+          <t>SUTURA DE HERIDA UNICA  EN AREA GENERAL</t>
         </is>
       </c>
       <c r="Q38" t="n">
@@ -3785,7 +3871,7 @@
     </row>
     <row r="39">
       <c r="A39" s="2" t="n">
-        <v>45967.57631627357</v>
+        <v>45967.79306267514</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
@@ -3804,19 +3890,27 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>TI</t>
+          <t>RC</t>
         </is>
       </c>
       <c r="F39" t="n">
-        <v>1063301201</v>
+        <v>1063314274</v>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>SHAIRA SAMIR MENDOZA MENESES</t>
-        </is>
-      </c>
-      <c r="H39" t="inlineStr"/>
-      <c r="I39" t="inlineStr"/>
+          <t>DAYLIN  CHAVEZ  CARE</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>3135496221</t>
+        </is>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>3135496221</t>
+        </is>
+      </c>
       <c r="J39" t="inlineStr">
         <is>
           <t>05/11/2025</t>
@@ -3824,12 +3918,12 @@
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>R509</t>
+          <t>N760</t>
         </is>
       </c>
       <c r="L39" t="inlineStr">
         <is>
-          <t>SANTIAGO  AGUDELO VILORIA</t>
+          <t>MAIRON ALDAHIR ANGULO CARVAJAL</t>
         </is>
       </c>
       <c r="M39" t="n">
@@ -3841,11 +3935,11 @@
         </is>
       </c>
       <c r="O39" t="n">
-        <v>906208</v>
+        <v>901305</v>
       </c>
       <c r="P39" t="inlineStr">
         <is>
-          <t>DENGUE  ANTICUERPOS IG M</t>
+          <t>EXAMEN DIRECTO PARA HONGOS KOH</t>
         </is>
       </c>
       <c r="Q39" t="n">
@@ -3868,7 +3962,7 @@
     </row>
     <row r="40">
       <c r="A40" s="2" t="n">
-        <v>45967.57631627434</v>
+        <v>45967.79306267514</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
@@ -3891,19 +3985,21 @@
         </is>
       </c>
       <c r="F40" t="n">
-        <v>1003337179</v>
+        <v>50998259</v>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>CARMEN   SEÑA GUERRA</t>
-        </is>
-      </c>
-      <c r="H40" t="n">
-        <v>3103963600</v>
+          <t>ENILSA DEL CARMEN DIAZ ARGUMEDO</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>3117507585</t>
+        </is>
       </c>
       <c r="I40" t="inlineStr">
         <is>
-          <t>3106765113</t>
+          <t>3147390742</t>
         </is>
       </c>
       <c r="J40" t="inlineStr">
@@ -3913,12 +4009,12 @@
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>R074</t>
+          <t>D179</t>
         </is>
       </c>
       <c r="L40" t="inlineStr">
         <is>
-          <t>DANIELA ALEXANDRA PEREZ CORDERO</t>
+          <t>EDGAR  ACOSTA GANDIA</t>
         </is>
       </c>
       <c r="M40" t="n">
@@ -3930,20 +4026,18 @@
         </is>
       </c>
       <c r="O40" t="n">
-        <v>906039</v>
+        <v>890235</v>
       </c>
       <c r="P40" t="inlineStr">
         <is>
-          <t>TREPONEMA PALLIDUM  - Prueba Rapida</t>
+          <t>CONSULTA DE PRIMERA VEZ POR ESPECIALISTA EN CIRUGÍA GENERAL</t>
         </is>
       </c>
       <c r="Q40" t="n">
         <v>1</v>
       </c>
       <c r="R40" t="inlineStr"/>
-      <c r="S40" t="n">
-        <v>0</v>
-      </c>
+      <c r="S40" t="inlineStr"/>
       <c r="T40" t="inlineStr"/>
       <c r="U40" t="inlineStr"/>
       <c r="V40" t="inlineStr"/>
@@ -3957,7 +4051,7 @@
     </row>
     <row r="41">
       <c r="A41" s="2" t="n">
-        <v>45967.57631627529</v>
+        <v>45967.79306267514</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
@@ -3980,19 +4074,21 @@
         </is>
       </c>
       <c r="F41" t="n">
-        <v>1003337179</v>
+        <v>78292216</v>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>CARMEN   SEÑA GUERRA</t>
-        </is>
-      </c>
-      <c r="H41" t="n">
-        <v>3103963600</v>
+          <t>HERNAN JOSE BETACUR RODRIGUEZ</t>
+        </is>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>3224208658</t>
+        </is>
       </c>
       <c r="I41" t="inlineStr">
         <is>
-          <t>3106765113</t>
+          <t>3224208658</t>
         </is>
       </c>
       <c r="J41" t="inlineStr">
@@ -4002,12 +4098,12 @@
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>R074</t>
+          <t>L309</t>
         </is>
       </c>
       <c r="L41" t="inlineStr">
         <is>
-          <t>DANIELA ALEXANDRA PEREZ CORDERO</t>
+          <t>MAIRON ALDAHIR ANGULO CARVAJAL</t>
         </is>
       </c>
       <c r="M41" t="n">
@@ -4019,11 +4115,11 @@
         </is>
       </c>
       <c r="O41" t="n">
-        <v>906249</v>
+        <v>890242</v>
       </c>
       <c r="P41" t="inlineStr">
         <is>
-          <t>VIH 1 Y 2  ANTICUERPOS PRUEBA RAPIDA</t>
+          <t>CONSULTA DE PRIMERA VEZ POR ESPECIALISTA EN DERMATOLOGÍA</t>
         </is>
       </c>
       <c r="Q41" t="n">
@@ -4046,7 +4142,7 @@
     </row>
     <row r="42">
       <c r="A42" s="2" t="n">
-        <v>45967.57631627608</v>
+        <v>45967.79306267514</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
@@ -4069,19 +4165,21 @@
         </is>
       </c>
       <c r="F42" t="n">
-        <v>22533915</v>
+        <v>1063284002</v>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>LEANA PATRICIA MUÑOZ JIMENEZ</t>
-        </is>
-      </c>
-      <c r="H42" t="n">
-        <v>3216702029</v>
+          <t>YORJANY MILENA TOVAR RAMOS</t>
+        </is>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>3147481140</t>
+        </is>
       </c>
       <c r="I42" t="inlineStr">
         <is>
-          <t>3156606596</t>
+          <t>3147481140</t>
         </is>
       </c>
       <c r="J42" t="inlineStr">
@@ -4091,12 +4189,12 @@
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>R074</t>
+          <t>N648</t>
         </is>
       </c>
       <c r="L42" t="inlineStr">
         <is>
-          <t>DANIELA ALEXANDRA PEREZ CORDERO</t>
+          <t>EDGAR  ACOSTA GANDIA</t>
         </is>
       </c>
       <c r="M42" t="n">
@@ -4108,11 +4206,11 @@
         </is>
       </c>
       <c r="O42" t="n">
-        <v>903801</v>
+        <v>881201</v>
       </c>
       <c r="P42" t="inlineStr">
         <is>
-          <t>ACIDO URICO O:P</t>
+          <t>ULTRASONOGRAFIA DIAGNOSTICA DE MAMA  CON TRANSDUCTOR DE 7 MHZ O MAS</t>
         </is>
       </c>
       <c r="Q42" t="n">
@@ -4135,7 +4233,7 @@
     </row>
     <row r="43">
       <c r="A43" s="2" t="n">
-        <v>45967.57631627684</v>
+        <v>45967.79306268667</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
@@ -4154,23 +4252,25 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>CC</t>
+          <t>TI</t>
         </is>
       </c>
       <c r="F43" t="n">
-        <v>22533915</v>
+        <v>1066604406</v>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>LEANA PATRICIA MUÑOZ JIMENEZ</t>
-        </is>
-      </c>
-      <c r="H43" t="n">
-        <v>3216702029</v>
+          <t>MATIAS   RODRIGUEZ HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>3137086677</t>
+        </is>
       </c>
       <c r="I43" t="inlineStr">
         <is>
-          <t>3156606596</t>
+          <t>3506517849</t>
         </is>
       </c>
       <c r="J43" t="inlineStr">
@@ -4180,12 +4280,12 @@
       </c>
       <c r="K43" t="inlineStr">
         <is>
-          <t>R074</t>
+          <t>E569</t>
         </is>
       </c>
       <c r="L43" t="inlineStr">
         <is>
-          <t>DANIELA ALEXANDRA PEREZ CORDERO</t>
+          <t>EDGAR  EMBUZ TORRALVO</t>
         </is>
       </c>
       <c r="M43" t="n">
@@ -4197,11 +4297,11 @@
         </is>
       </c>
       <c r="O43" t="n">
-        <v>906914</v>
+        <v>904902</v>
       </c>
       <c r="P43" t="inlineStr">
         <is>
-          <t>PROTEÍNA C REACTIVA  PRUEBA SEMICUANTITATIVA</t>
+          <t>HORMONA ESTIMULANTE DEL TIROIDES TSH</t>
         </is>
       </c>
       <c r="Q43" t="n">
@@ -4224,7 +4324,7 @@
     </row>
     <row r="44">
       <c r="A44" s="2" t="n">
-        <v>45967.57631627761</v>
+        <v>45967.79306268667</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
@@ -4243,23 +4343,25 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>CC</t>
+          <t>TI</t>
         </is>
       </c>
       <c r="F44" t="n">
-        <v>22533915</v>
+        <v>1066604406</v>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>LEANA PATRICIA MUÑOZ JIMENEZ</t>
-        </is>
-      </c>
-      <c r="H44" t="n">
-        <v>3216702029</v>
+          <t>MATIAS   RODRIGUEZ HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>3137086677</t>
+        </is>
       </c>
       <c r="I44" t="inlineStr">
         <is>
-          <t>3156606596</t>
+          <t>3506517849</t>
         </is>
       </c>
       <c r="J44" t="inlineStr">
@@ -4269,12 +4371,12 @@
       </c>
       <c r="K44" t="inlineStr">
         <is>
-          <t>R074</t>
+          <t>E569</t>
         </is>
       </c>
       <c r="L44" t="inlineStr">
         <is>
-          <t>DANIELA ALEXANDRA PEREZ CORDERO</t>
+          <t>EDGAR  EMBUZ TORRALVO</t>
         </is>
       </c>
       <c r="M44" t="n">
@@ -4286,11 +4388,11 @@
         </is>
       </c>
       <c r="O44" t="n">
-        <v>906914</v>
+        <v>904921</v>
       </c>
       <c r="P44" t="inlineStr">
         <is>
-          <t>PROTEÍNA C REACTIVA  PRUEBA SEMICUANTITATIVA</t>
+          <t>TIROXINA LIBRE T4L</t>
         </is>
       </c>
       <c r="Q44" t="n">
@@ -4313,7 +4415,7 @@
     </row>
     <row r="45">
       <c r="A45" s="2" t="n">
-        <v>45967.57631627838</v>
+        <v>45967.79306268667</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
@@ -4336,19 +4438,21 @@
         </is>
       </c>
       <c r="F45" t="n">
-        <v>1017148528</v>
+        <v>26000441</v>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>TANIA ROSA ARGUMEDO MADERA</t>
-        </is>
-      </c>
-      <c r="H45" t="n">
-        <v>3106303540</v>
+          <t>LILIANA DEL CARMEN MARTINEZ UPARELA</t>
+        </is>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>3135627000</t>
+        </is>
       </c>
       <c r="I45" t="inlineStr">
         <is>
-          <t>3116800494</t>
+          <t>3135627000</t>
         </is>
       </c>
       <c r="J45" t="inlineStr">
@@ -4358,12 +4462,12 @@
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>Z008</t>
+          <t>R609</t>
         </is>
       </c>
       <c r="L45" t="inlineStr">
         <is>
-          <t>EDGAR  ACOSTA GANDIA</t>
+          <t>DAILIN ALEXANDRA MENDOZA GUTIERREZ</t>
         </is>
       </c>
       <c r="M45" t="n">
@@ -4386,7 +4490,9 @@
         <v>1</v>
       </c>
       <c r="R45" t="inlineStr"/>
-      <c r="S45" t="inlineStr"/>
+      <c r="S45" t="n">
+        <v>0</v>
+      </c>
       <c r="T45" t="inlineStr"/>
       <c r="U45" t="inlineStr"/>
       <c r="V45" t="inlineStr"/>
@@ -4400,7 +4506,7 @@
     </row>
     <row r="46">
       <c r="A46" s="2" t="n">
-        <v>45967.57631627914</v>
+        <v>45967.79306268667</v>
       </c>
       <c r="B46" t="inlineStr">
         <is>
@@ -4423,19 +4529,21 @@
         </is>
       </c>
       <c r="F46" t="n">
-        <v>25989944</v>
+        <v>26000441</v>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>AMADA ISABEL CERVANTES MARTINEZ</t>
-        </is>
-      </c>
-      <c r="H46" t="n">
-        <v>3122241872</v>
+          <t>LILIANA DEL CARMEN MARTINEZ UPARELA</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>3135627000</t>
+        </is>
       </c>
       <c r="I46" t="inlineStr">
         <is>
-          <t>3226221101</t>
+          <t>3135627000</t>
         </is>
       </c>
       <c r="J46" t="inlineStr">
@@ -4445,26 +4553,28 @@
       </c>
       <c r="K46" t="inlineStr">
         <is>
-          <t>I10X</t>
+          <t>R609</t>
         </is>
       </c>
       <c r="L46" t="inlineStr">
         <is>
-          <t>JASDANYS  SAENZ MEDRANO</t>
-        </is>
-      </c>
-      <c r="M46" t="inlineStr"/>
+          <t>DAILIN ALEXANDRA MENDOZA GUTIERREZ</t>
+        </is>
+      </c>
+      <c r="M46" t="n">
+        <v>78</v>
+      </c>
       <c r="N46" t="inlineStr">
         <is>
-          <t>PYP MEDICO</t>
+          <t>MEDICINA GENERAL</t>
         </is>
       </c>
       <c r="O46" t="n">
-        <v>903026</v>
+        <v>903869</v>
       </c>
       <c r="P46" t="inlineStr">
         <is>
-          <t>MICROALBUMINURIA POR EIA</t>
+          <t>UREA</t>
         </is>
       </c>
       <c r="Q46" t="n">
@@ -4487,7 +4597,7 @@
     </row>
     <row r="47">
       <c r="A47" s="2" t="n">
-        <v>45967.5763162799</v>
+        <v>45967.79306269752</v>
       </c>
       <c r="B47" t="inlineStr">
         <is>
@@ -4506,23 +4616,25 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>TI</t>
+          <t>CC</t>
         </is>
       </c>
       <c r="F47" t="n">
-        <v>1066605496</v>
+        <v>26000441</v>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>WILLIAM JOSE PADRON MONTES</t>
-        </is>
-      </c>
-      <c r="H47" t="n">
-        <v>3006352654</v>
+          <t>LILIANA DEL CARMEN MARTINEZ UPARELA</t>
+        </is>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>3135627000</t>
+        </is>
       </c>
       <c r="I47" t="inlineStr">
         <is>
-          <t>3008161877</t>
+          <t>3135627000</t>
         </is>
       </c>
       <c r="J47" t="inlineStr">
@@ -4532,12 +4644,12 @@
       </c>
       <c r="K47" t="inlineStr">
         <is>
-          <t>S411</t>
+          <t>R609</t>
         </is>
       </c>
       <c r="L47" t="inlineStr">
         <is>
-          <t>PAOLA CRISTINA HERAZO MIRANDA</t>
+          <t>DAILIN ALEXANDRA MENDOZA GUTIERREZ</t>
         </is>
       </c>
       <c r="M47" t="n">
@@ -4549,11 +4661,11 @@
         </is>
       </c>
       <c r="O47" t="n">
-        <v>865101</v>
+        <v>906466</v>
       </c>
       <c r="P47" t="inlineStr">
         <is>
-          <t>SUTURA DE HERIDA UNICA  EN AREA GENERAL</t>
+          <t>CITRULINA ANTICUERPO (ANTI PEPTIDO CICLICO  CITRULINADO O SEMIAUTOMATIZADO O AUTOMATIZADO)</t>
         </is>
       </c>
       <c r="Q47" t="n">
@@ -4576,7 +4688,7 @@
     </row>
     <row r="48">
       <c r="A48" s="2" t="n">
-        <v>45967.57631628066</v>
+        <v>45967.79306269752</v>
       </c>
       <c r="B48" t="inlineStr">
         <is>
@@ -4595,23 +4707,25 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>RC</t>
+          <t>CC</t>
         </is>
       </c>
       <c r="F48" t="n">
-        <v>1063314274</v>
+        <v>26000441</v>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>DAYLIN  CHAVEZ  CARE</t>
-        </is>
-      </c>
-      <c r="H48" t="n">
-        <v>3135496221</v>
+          <t>LILIANA DEL CARMEN MARTINEZ UPARELA</t>
+        </is>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>3135627000</t>
+        </is>
       </c>
       <c r="I48" t="inlineStr">
         <is>
-          <t>3135496221</t>
+          <t>3135627000</t>
         </is>
       </c>
       <c r="J48" t="inlineStr">
@@ -4621,12 +4735,12 @@
       </c>
       <c r="K48" t="inlineStr">
         <is>
-          <t>N760</t>
+          <t>R609</t>
         </is>
       </c>
       <c r="L48" t="inlineStr">
         <is>
-          <t>MAIRON ALDAHIR ANGULO CARVAJAL</t>
+          <t>DAILIN ALEXANDRA MENDOZA GUTIERREZ</t>
         </is>
       </c>
       <c r="M48" t="n">
@@ -4638,11 +4752,11 @@
         </is>
       </c>
       <c r="O48" t="n">
-        <v>901305</v>
+        <v>906911</v>
       </c>
       <c r="P48" t="inlineStr">
         <is>
-          <t>EXAMEN DIRECTO PARA HONGOS KOH</t>
+          <t>FACTOR REMATOIDEO R.A. SEMICUANTITATIVO POR LÁTEX</t>
         </is>
       </c>
       <c r="Q48" t="n">
@@ -4665,7 +4779,7 @@
     </row>
     <row r="49">
       <c r="A49" s="2" t="n">
-        <v>45967.57631628141</v>
+        <v>45967.79306269752</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
@@ -4688,19 +4802,21 @@
         </is>
       </c>
       <c r="F49" t="n">
-        <v>50998259</v>
+        <v>1063283218</v>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>ENILSA DEL CARMEN DIAZ ARGUMEDO</t>
-        </is>
-      </c>
-      <c r="H49" t="n">
-        <v>3117507585</v>
+          <t>MALBIRIS DEL CARMEN PEÑA BALTAZAR</t>
+        </is>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>3116712888</t>
+        </is>
       </c>
       <c r="I49" t="inlineStr">
         <is>
-          <t>3147390742</t>
+          <t>3116712888</t>
         </is>
       </c>
       <c r="J49" t="inlineStr">
@@ -4710,7 +4826,7 @@
       </c>
       <c r="K49" t="inlineStr">
         <is>
-          <t>D179</t>
+          <t>Z008</t>
         </is>
       </c>
       <c r="L49" t="inlineStr">
@@ -4727,11 +4843,11 @@
         </is>
       </c>
       <c r="O49" t="n">
-        <v>890235</v>
+        <v>890376</v>
       </c>
       <c r="P49" t="inlineStr">
         <is>
-          <t>CONSULTA DE PRIMERA VEZ POR ESPECIALISTA EN CIRUGÍA GENERAL</t>
+          <t>CONSULTA DE CONTROL O DE SEGUIMIENTO POR ESPECIALISTA EN OFTALMOLOGIA</t>
         </is>
       </c>
       <c r="Q49" t="n">
@@ -4752,7 +4868,7 @@
     </row>
     <row r="50">
       <c r="A50" s="2" t="n">
-        <v>45967.57631628217</v>
+        <v>45967.79306270931</v>
       </c>
       <c r="B50" t="inlineStr">
         <is>
@@ -4775,19 +4891,21 @@
         </is>
       </c>
       <c r="F50" t="n">
-        <v>25987625</v>
+        <v>1063283218</v>
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>ROSA  DE LA ROSA SUAREZ</t>
-        </is>
-      </c>
-      <c r="H50" t="n">
-        <v>3102173742</v>
+          <t>MALBIRIS DEL CARMEN PEÑA BALTAZAR</t>
+        </is>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>3116712888</t>
+        </is>
       </c>
       <c r="I50" t="inlineStr">
         <is>
-          <t>3232892378</t>
+          <t>3116712888</t>
         </is>
       </c>
       <c r="J50" t="inlineStr">
@@ -4797,35 +4915,35 @@
       </c>
       <c r="K50" t="inlineStr">
         <is>
-          <t>I10X</t>
+          <t>Z008</t>
         </is>
       </c>
       <c r="L50" t="inlineStr">
         <is>
-          <t>JASDANYS  SAENZ MEDRANO</t>
-        </is>
-      </c>
-      <c r="M50" t="inlineStr"/>
+          <t>EDGAR  ACOSTA GANDIA</t>
+        </is>
+      </c>
+      <c r="M50" t="n">
+        <v>78</v>
+      </c>
       <c r="N50" t="inlineStr">
         <is>
-          <t>PYP MEDICO</t>
+          <t>MEDICINA GENERAL</t>
         </is>
       </c>
       <c r="O50" t="n">
-        <v>903026</v>
+        <v>902206</v>
       </c>
       <c r="P50" t="inlineStr">
         <is>
-          <t>MICROALBUMINURIA POR EIA</t>
+          <t>EXTENDIDO DE SANGRE PERIFERICA  ESTUDIO DE MORFOLOGIA</t>
         </is>
       </c>
       <c r="Q50" t="n">
         <v>1</v>
       </c>
       <c r="R50" t="inlineStr"/>
-      <c r="S50" t="n">
-        <v>0</v>
-      </c>
+      <c r="S50" t="inlineStr"/>
       <c r="T50" t="inlineStr"/>
       <c r="U50" t="inlineStr"/>
       <c r="V50" t="inlineStr"/>
@@ -4839,7 +4957,7 @@
     </row>
     <row r="51">
       <c r="A51" s="2" t="n">
-        <v>45967.57631628292</v>
+        <v>45967.79306270931</v>
       </c>
       <c r="B51" t="inlineStr">
         <is>
@@ -4862,19 +4980,21 @@
         </is>
       </c>
       <c r="F51" t="n">
-        <v>78292216</v>
+        <v>1063283218</v>
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>HERNAN JOSE BETACUR RODRIGUEZ</t>
-        </is>
-      </c>
-      <c r="H51" t="n">
-        <v>3224208658</v>
+          <t>MALBIRIS DEL CARMEN PEÑA BALTAZAR</t>
+        </is>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>3116712888</t>
+        </is>
       </c>
       <c r="I51" t="inlineStr">
         <is>
-          <t>3224208658</t>
+          <t>3116712888</t>
         </is>
       </c>
       <c r="J51" t="inlineStr">
@@ -4884,12 +5004,12 @@
       </c>
       <c r="K51" t="inlineStr">
         <is>
-          <t>L309</t>
+          <t>Z008</t>
         </is>
       </c>
       <c r="L51" t="inlineStr">
         <is>
-          <t>MAIRON ALDAHIR ANGULO CARVAJAL</t>
+          <t>EDGAR  ACOSTA GANDIA</t>
         </is>
       </c>
       <c r="M51" t="n">
@@ -4901,20 +5021,18 @@
         </is>
       </c>
       <c r="O51" t="n">
-        <v>890242</v>
+        <v>903801</v>
       </c>
       <c r="P51" t="inlineStr">
         <is>
-          <t>CONSULTA DE PRIMERA VEZ POR ESPECIALISTA EN DERMATOLOGÍA</t>
+          <t>ACIDO URICO O:P</t>
         </is>
       </c>
       <c r="Q51" t="n">
         <v>1</v>
       </c>
       <c r="R51" t="inlineStr"/>
-      <c r="S51" t="n">
-        <v>0</v>
-      </c>
+      <c r="S51" t="inlineStr"/>
       <c r="T51" t="inlineStr"/>
       <c r="U51" t="inlineStr"/>
       <c r="V51" t="inlineStr"/>
@@ -4928,7 +5046,7 @@
     </row>
     <row r="52">
       <c r="A52" s="2" t="n">
-        <v>45967.57631628367</v>
+        <v>45967.79306272101</v>
       </c>
       <c r="B52" t="inlineStr">
         <is>
@@ -4951,19 +5069,21 @@
         </is>
       </c>
       <c r="F52" t="n">
-        <v>1063284002</v>
+        <v>9114171</v>
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>YORJANY MILENA TOVAR RAMOS</t>
-        </is>
-      </c>
-      <c r="H52" t="n">
-        <v>3147481140</v>
+          <t>FELIX SEGUNDO BERRIO MERCADO</t>
+        </is>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>3001900997</t>
+        </is>
       </c>
       <c r="I52" t="inlineStr">
         <is>
-          <t>3147481140</t>
+          <t>3126663905</t>
         </is>
       </c>
       <c r="J52" t="inlineStr">
@@ -4973,12 +5093,12 @@
       </c>
       <c r="K52" t="inlineStr">
         <is>
-          <t>N648</t>
+          <t>D106</t>
         </is>
       </c>
       <c r="L52" t="inlineStr">
         <is>
-          <t>EDGAR  ACOSTA GANDIA</t>
+          <t>CAMILA JOHANA PACITO DIAZ</t>
         </is>
       </c>
       <c r="M52" t="n">
@@ -4990,11 +5110,11 @@
         </is>
       </c>
       <c r="O52" t="n">
-        <v>881201</v>
+        <v>906610</v>
       </c>
       <c r="P52" t="inlineStr">
         <is>
-          <t>ULTRASONOGRAFIA DIAGNOSTICA DE MAMA  CON TRANSDUCTOR DE 7 MHZ O MAS</t>
+          <t>ANTIGENO ESPECIFICO DE PROSTATA PSA</t>
         </is>
       </c>
       <c r="Q52" t="n">
@@ -5017,7 +5137,7 @@
     </row>
     <row r="53">
       <c r="A53" s="2" t="n">
-        <v>45967.57631628445</v>
+        <v>45967.79306272101</v>
       </c>
       <c r="B53" t="inlineStr">
         <is>
@@ -5036,23 +5156,25 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>TI</t>
+          <t>RC</t>
         </is>
       </c>
       <c r="F53" t="n">
-        <v>1066604406</v>
+        <v>1063311559</v>
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>MATIAS   RODRIGUEZ HERNANDEZ</t>
-        </is>
-      </c>
-      <c r="H53" t="n">
-        <v>3137086677</v>
+          <t>DIDIER  CERVANTES FLOREZ</t>
+        </is>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>3113449253</t>
+        </is>
       </c>
       <c r="I53" t="inlineStr">
         <is>
-          <t>3506517849</t>
+          <t>3126969937</t>
         </is>
       </c>
       <c r="J53" t="inlineStr">
@@ -5062,12 +5184,12 @@
       </c>
       <c r="K53" t="inlineStr">
         <is>
-          <t>E569</t>
+          <t>S819</t>
         </is>
       </c>
       <c r="L53" t="inlineStr">
         <is>
-          <t>EDGAR  EMBUZ TORRALVO</t>
+          <t>NICOLAS  MARTINEZ MACEA</t>
         </is>
       </c>
       <c r="M53" t="n">
@@ -5079,11 +5201,11 @@
         </is>
       </c>
       <c r="O53" t="n">
-        <v>904902</v>
+        <v>865101</v>
       </c>
       <c r="P53" t="inlineStr">
         <is>
-          <t>HORMONA ESTIMULANTE DEL TIROIDES TSH</t>
+          <t>SUTURA DE HERIDA UNICA  EN AREA GENERAL</t>
         </is>
       </c>
       <c r="Q53" t="n">
@@ -5104,977 +5226,6 @@
         </is>
       </c>
     </row>
-    <row r="54">
-      <c r="A54" s="2" t="n">
-        <v>45967.57631628521</v>
-      </c>
-      <c r="B54" t="inlineStr">
-        <is>
-          <t>812000344</t>
-        </is>
-      </c>
-      <c r="C54" t="inlineStr">
-        <is>
-          <t>11033</t>
-        </is>
-      </c>
-      <c r="D54" t="inlineStr">
-        <is>
-          <t>ESE HOSPITAL LOCAL DE MONTELIBANO</t>
-        </is>
-      </c>
-      <c r="E54" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="F54" t="n">
-        <v>1066604406</v>
-      </c>
-      <c r="G54" t="inlineStr">
-        <is>
-          <t>MATIAS   RODRIGUEZ HERNANDEZ</t>
-        </is>
-      </c>
-      <c r="H54" t="n">
-        <v>3137086677</v>
-      </c>
-      <c r="I54" t="inlineStr">
-        <is>
-          <t>3506517849</t>
-        </is>
-      </c>
-      <c r="J54" t="inlineStr">
-        <is>
-          <t>05/11/2025</t>
-        </is>
-      </c>
-      <c r="K54" t="inlineStr">
-        <is>
-          <t>E569</t>
-        </is>
-      </c>
-      <c r="L54" t="inlineStr">
-        <is>
-          <t>EDGAR  EMBUZ TORRALVO</t>
-        </is>
-      </c>
-      <c r="M54" t="n">
-        <v>78</v>
-      </c>
-      <c r="N54" t="inlineStr">
-        <is>
-          <t>MEDICINA GENERAL</t>
-        </is>
-      </c>
-      <c r="O54" t="n">
-        <v>904921</v>
-      </c>
-      <c r="P54" t="inlineStr">
-        <is>
-          <t>TIROXINA LIBRE T4L</t>
-        </is>
-      </c>
-      <c r="Q54" t="n">
-        <v>1</v>
-      </c>
-      <c r="R54" t="inlineStr"/>
-      <c r="S54" t="n">
-        <v>0</v>
-      </c>
-      <c r="T54" t="inlineStr"/>
-      <c r="U54" t="inlineStr"/>
-      <c r="V54" t="inlineStr"/>
-      <c r="W54" t="inlineStr"/>
-      <c r="X54" t="inlineStr"/>
-      <c r="Y54" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" s="2" t="n">
-        <v>45967.57631628596</v>
-      </c>
-      <c r="B55" t="inlineStr">
-        <is>
-          <t>812000344</t>
-        </is>
-      </c>
-      <c r="C55" t="inlineStr">
-        <is>
-          <t>11033</t>
-        </is>
-      </c>
-      <c r="D55" t="inlineStr">
-        <is>
-          <t>ESE HOSPITAL LOCAL DE MONTELIBANO</t>
-        </is>
-      </c>
-      <c r="E55" t="inlineStr">
-        <is>
-          <t>CC</t>
-        </is>
-      </c>
-      <c r="F55" t="n">
-        <v>26000441</v>
-      </c>
-      <c r="G55" t="inlineStr">
-        <is>
-          <t>LILIANA DEL CARMEN MARTINEZ UPARELA</t>
-        </is>
-      </c>
-      <c r="H55" t="n">
-        <v>3135627000</v>
-      </c>
-      <c r="I55" t="inlineStr">
-        <is>
-          <t>3135627000</t>
-        </is>
-      </c>
-      <c r="J55" t="inlineStr">
-        <is>
-          <t>05/11/2025</t>
-        </is>
-      </c>
-      <c r="K55" t="inlineStr">
-        <is>
-          <t>R609</t>
-        </is>
-      </c>
-      <c r="L55" t="inlineStr">
-        <is>
-          <t>DAILIN ALEXANDRA MENDOZA GUTIERREZ</t>
-        </is>
-      </c>
-      <c r="M55" t="n">
-        <v>78</v>
-      </c>
-      <c r="N55" t="inlineStr">
-        <is>
-          <t>MEDICINA GENERAL</t>
-        </is>
-      </c>
-      <c r="O55" t="n">
-        <v>903801</v>
-      </c>
-      <c r="P55" t="inlineStr">
-        <is>
-          <t>ACIDO URICO O:P</t>
-        </is>
-      </c>
-      <c r="Q55" t="n">
-        <v>1</v>
-      </c>
-      <c r="R55" t="inlineStr"/>
-      <c r="S55" t="n">
-        <v>0</v>
-      </c>
-      <c r="T55" t="inlineStr"/>
-      <c r="U55" t="inlineStr"/>
-      <c r="V55" t="inlineStr"/>
-      <c r="W55" t="inlineStr"/>
-      <c r="X55" t="inlineStr"/>
-      <c r="Y55" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" s="2" t="n">
-        <v>45967.57631628692</v>
-      </c>
-      <c r="B56" t="inlineStr">
-        <is>
-          <t>812000344</t>
-        </is>
-      </c>
-      <c r="C56" t="inlineStr">
-        <is>
-          <t>11033</t>
-        </is>
-      </c>
-      <c r="D56" t="inlineStr">
-        <is>
-          <t>ESE HOSPITAL LOCAL DE MONTELIBANO</t>
-        </is>
-      </c>
-      <c r="E56" t="inlineStr">
-        <is>
-          <t>CC</t>
-        </is>
-      </c>
-      <c r="F56" t="n">
-        <v>26000441</v>
-      </c>
-      <c r="G56" t="inlineStr">
-        <is>
-          <t>LILIANA DEL CARMEN MARTINEZ UPARELA</t>
-        </is>
-      </c>
-      <c r="H56" t="n">
-        <v>3135627000</v>
-      </c>
-      <c r="I56" t="inlineStr">
-        <is>
-          <t>3135627000</t>
-        </is>
-      </c>
-      <c r="J56" t="inlineStr">
-        <is>
-          <t>05/11/2025</t>
-        </is>
-      </c>
-      <c r="K56" t="inlineStr">
-        <is>
-          <t>R609</t>
-        </is>
-      </c>
-      <c r="L56" t="inlineStr">
-        <is>
-          <t>DAILIN ALEXANDRA MENDOZA GUTIERREZ</t>
-        </is>
-      </c>
-      <c r="M56" t="n">
-        <v>78</v>
-      </c>
-      <c r="N56" t="inlineStr">
-        <is>
-          <t>MEDICINA GENERAL</t>
-        </is>
-      </c>
-      <c r="O56" t="n">
-        <v>903869</v>
-      </c>
-      <c r="P56" t="inlineStr">
-        <is>
-          <t>UREA</t>
-        </is>
-      </c>
-      <c r="Q56" t="n">
-        <v>1</v>
-      </c>
-      <c r="R56" t="inlineStr"/>
-      <c r="S56" t="n">
-        <v>0</v>
-      </c>
-      <c r="T56" t="inlineStr"/>
-      <c r="U56" t="inlineStr"/>
-      <c r="V56" t="inlineStr"/>
-      <c r="W56" t="inlineStr"/>
-      <c r="X56" t="inlineStr"/>
-      <c r="Y56" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" s="2" t="n">
-        <v>45967.57631628773</v>
-      </c>
-      <c r="B57" t="inlineStr">
-        <is>
-          <t>812000344</t>
-        </is>
-      </c>
-      <c r="C57" t="inlineStr">
-        <is>
-          <t>11033</t>
-        </is>
-      </c>
-      <c r="D57" t="inlineStr">
-        <is>
-          <t>ESE HOSPITAL LOCAL DE MONTELIBANO</t>
-        </is>
-      </c>
-      <c r="E57" t="inlineStr">
-        <is>
-          <t>CC</t>
-        </is>
-      </c>
-      <c r="F57" t="n">
-        <v>26000441</v>
-      </c>
-      <c r="G57" t="inlineStr">
-        <is>
-          <t>LILIANA DEL CARMEN MARTINEZ UPARELA</t>
-        </is>
-      </c>
-      <c r="H57" t="n">
-        <v>3135627000</v>
-      </c>
-      <c r="I57" t="inlineStr">
-        <is>
-          <t>3135627000</t>
-        </is>
-      </c>
-      <c r="J57" t="inlineStr">
-        <is>
-          <t>05/11/2025</t>
-        </is>
-      </c>
-      <c r="K57" t="inlineStr">
-        <is>
-          <t>R609</t>
-        </is>
-      </c>
-      <c r="L57" t="inlineStr">
-        <is>
-          <t>DAILIN ALEXANDRA MENDOZA GUTIERREZ</t>
-        </is>
-      </c>
-      <c r="M57" t="n">
-        <v>78</v>
-      </c>
-      <c r="N57" t="inlineStr">
-        <is>
-          <t>MEDICINA GENERAL</t>
-        </is>
-      </c>
-      <c r="O57" t="n">
-        <v>906466</v>
-      </c>
-      <c r="P57" t="inlineStr">
-        <is>
-          <t>CITRULINA ANTICUERPO (ANTI PEPTIDO CICLICO  CITRULINADO O SEMIAUTOMATIZADO O AUTOMATIZADO)</t>
-        </is>
-      </c>
-      <c r="Q57" t="n">
-        <v>1</v>
-      </c>
-      <c r="R57" t="inlineStr"/>
-      <c r="S57" t="n">
-        <v>0</v>
-      </c>
-      <c r="T57" t="inlineStr"/>
-      <c r="U57" t="inlineStr"/>
-      <c r="V57" t="inlineStr"/>
-      <c r="W57" t="inlineStr"/>
-      <c r="X57" t="inlineStr"/>
-      <c r="Y57" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" s="2" t="n">
-        <v>45967.57631628848</v>
-      </c>
-      <c r="B58" t="inlineStr">
-        <is>
-          <t>812000344</t>
-        </is>
-      </c>
-      <c r="C58" t="inlineStr">
-        <is>
-          <t>11033</t>
-        </is>
-      </c>
-      <c r="D58" t="inlineStr">
-        <is>
-          <t>ESE HOSPITAL LOCAL DE MONTELIBANO</t>
-        </is>
-      </c>
-      <c r="E58" t="inlineStr">
-        <is>
-          <t>CC</t>
-        </is>
-      </c>
-      <c r="F58" t="n">
-        <v>26000441</v>
-      </c>
-      <c r="G58" t="inlineStr">
-        <is>
-          <t>LILIANA DEL CARMEN MARTINEZ UPARELA</t>
-        </is>
-      </c>
-      <c r="H58" t="n">
-        <v>3135627000</v>
-      </c>
-      <c r="I58" t="inlineStr">
-        <is>
-          <t>3135627000</t>
-        </is>
-      </c>
-      <c r="J58" t="inlineStr">
-        <is>
-          <t>05/11/2025</t>
-        </is>
-      </c>
-      <c r="K58" t="inlineStr">
-        <is>
-          <t>R609</t>
-        </is>
-      </c>
-      <c r="L58" t="inlineStr">
-        <is>
-          <t>DAILIN ALEXANDRA MENDOZA GUTIERREZ</t>
-        </is>
-      </c>
-      <c r="M58" t="n">
-        <v>78</v>
-      </c>
-      <c r="N58" t="inlineStr">
-        <is>
-          <t>MEDICINA GENERAL</t>
-        </is>
-      </c>
-      <c r="O58" t="n">
-        <v>906911</v>
-      </c>
-      <c r="P58" t="inlineStr">
-        <is>
-          <t>FACTOR REMATOIDEO R.A. SEMICUANTITATIVO POR LÁTEX</t>
-        </is>
-      </c>
-      <c r="Q58" t="n">
-        <v>1</v>
-      </c>
-      <c r="R58" t="inlineStr"/>
-      <c r="S58" t="n">
-        <v>0</v>
-      </c>
-      <c r="T58" t="inlineStr"/>
-      <c r="U58" t="inlineStr"/>
-      <c r="V58" t="inlineStr"/>
-      <c r="W58" t="inlineStr"/>
-      <c r="X58" t="inlineStr"/>
-      <c r="Y58" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" s="2" t="n">
-        <v>45967.57631628925</v>
-      </c>
-      <c r="B59" t="inlineStr">
-        <is>
-          <t>812000344</t>
-        </is>
-      </c>
-      <c r="C59" t="inlineStr">
-        <is>
-          <t>11033</t>
-        </is>
-      </c>
-      <c r="D59" t="inlineStr">
-        <is>
-          <t>ESE HOSPITAL LOCAL DE MONTELIBANO</t>
-        </is>
-      </c>
-      <c r="E59" t="inlineStr">
-        <is>
-          <t>CC</t>
-        </is>
-      </c>
-      <c r="F59" t="n">
-        <v>1063283218</v>
-      </c>
-      <c r="G59" t="inlineStr">
-        <is>
-          <t>MALBIRIS DEL CARMEN PEÑA BALTAZAR</t>
-        </is>
-      </c>
-      <c r="H59" t="n">
-        <v>3116712888</v>
-      </c>
-      <c r="I59" t="inlineStr">
-        <is>
-          <t>3116712888</t>
-        </is>
-      </c>
-      <c r="J59" t="inlineStr">
-        <is>
-          <t>05/11/2025</t>
-        </is>
-      </c>
-      <c r="K59" t="inlineStr">
-        <is>
-          <t>Z008</t>
-        </is>
-      </c>
-      <c r="L59" t="inlineStr">
-        <is>
-          <t>EDGAR  ACOSTA GANDIA</t>
-        </is>
-      </c>
-      <c r="M59" t="n">
-        <v>78</v>
-      </c>
-      <c r="N59" t="inlineStr">
-        <is>
-          <t>MEDICINA GENERAL</t>
-        </is>
-      </c>
-      <c r="O59" t="n">
-        <v>890376</v>
-      </c>
-      <c r="P59" t="inlineStr">
-        <is>
-          <t>CONSULTA DE CONTROL O DE SEGUIMIENTO POR ESPECIALISTA EN OFTALMOLOGIA</t>
-        </is>
-      </c>
-      <c r="Q59" t="n">
-        <v>1</v>
-      </c>
-      <c r="R59" t="inlineStr"/>
-      <c r="S59" t="inlineStr"/>
-      <c r="T59" t="inlineStr"/>
-      <c r="U59" t="inlineStr"/>
-      <c r="V59" t="inlineStr"/>
-      <c r="W59" t="inlineStr"/>
-      <c r="X59" t="inlineStr"/>
-      <c r="Y59" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" s="2" t="n">
-        <v>45967.57631629</v>
-      </c>
-      <c r="B60" t="inlineStr">
-        <is>
-          <t>812000344</t>
-        </is>
-      </c>
-      <c r="C60" t="inlineStr">
-        <is>
-          <t>11033</t>
-        </is>
-      </c>
-      <c r="D60" t="inlineStr">
-        <is>
-          <t>ESE HOSPITAL LOCAL DE MONTELIBANO</t>
-        </is>
-      </c>
-      <c r="E60" t="inlineStr">
-        <is>
-          <t>CC</t>
-        </is>
-      </c>
-      <c r="F60" t="n">
-        <v>1063283218</v>
-      </c>
-      <c r="G60" t="inlineStr">
-        <is>
-          <t>MALBIRIS DEL CARMEN PEÑA BALTAZAR</t>
-        </is>
-      </c>
-      <c r="H60" t="n">
-        <v>3116712888</v>
-      </c>
-      <c r="I60" t="inlineStr">
-        <is>
-          <t>3116712888</t>
-        </is>
-      </c>
-      <c r="J60" t="inlineStr">
-        <is>
-          <t>05/11/2025</t>
-        </is>
-      </c>
-      <c r="K60" t="inlineStr">
-        <is>
-          <t>Z008</t>
-        </is>
-      </c>
-      <c r="L60" t="inlineStr">
-        <is>
-          <t>EDGAR  ACOSTA GANDIA</t>
-        </is>
-      </c>
-      <c r="M60" t="n">
-        <v>78</v>
-      </c>
-      <c r="N60" t="inlineStr">
-        <is>
-          <t>MEDICINA GENERAL</t>
-        </is>
-      </c>
-      <c r="O60" t="n">
-        <v>902206</v>
-      </c>
-      <c r="P60" t="inlineStr">
-        <is>
-          <t>EXTENDIDO DE SANGRE PERIFERICA  ESTUDIO DE MORFOLOGIA</t>
-        </is>
-      </c>
-      <c r="Q60" t="n">
-        <v>1</v>
-      </c>
-      <c r="R60" t="inlineStr"/>
-      <c r="S60" t="inlineStr"/>
-      <c r="T60" t="inlineStr"/>
-      <c r="U60" t="inlineStr"/>
-      <c r="V60" t="inlineStr"/>
-      <c r="W60" t="inlineStr"/>
-      <c r="X60" t="inlineStr"/>
-      <c r="Y60" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" s="2" t="n">
-        <v>45967.57631629074</v>
-      </c>
-      <c r="B61" t="inlineStr">
-        <is>
-          <t>812000344</t>
-        </is>
-      </c>
-      <c r="C61" t="inlineStr">
-        <is>
-          <t>11033</t>
-        </is>
-      </c>
-      <c r="D61" t="inlineStr">
-        <is>
-          <t>ESE HOSPITAL LOCAL DE MONTELIBANO</t>
-        </is>
-      </c>
-      <c r="E61" t="inlineStr">
-        <is>
-          <t>CC</t>
-        </is>
-      </c>
-      <c r="F61" t="n">
-        <v>1063283218</v>
-      </c>
-      <c r="G61" t="inlineStr">
-        <is>
-          <t>MALBIRIS DEL CARMEN PEÑA BALTAZAR</t>
-        </is>
-      </c>
-      <c r="H61" t="n">
-        <v>3116712888</v>
-      </c>
-      <c r="I61" t="inlineStr">
-        <is>
-          <t>3116712888</t>
-        </is>
-      </c>
-      <c r="J61" t="inlineStr">
-        <is>
-          <t>05/11/2025</t>
-        </is>
-      </c>
-      <c r="K61" t="inlineStr">
-        <is>
-          <t>Z008</t>
-        </is>
-      </c>
-      <c r="L61" t="inlineStr">
-        <is>
-          <t>EDGAR  ACOSTA GANDIA</t>
-        </is>
-      </c>
-      <c r="M61" t="n">
-        <v>78</v>
-      </c>
-      <c r="N61" t="inlineStr">
-        <is>
-          <t>MEDICINA GENERAL</t>
-        </is>
-      </c>
-      <c r="O61" t="n">
-        <v>903801</v>
-      </c>
-      <c r="P61" t="inlineStr">
-        <is>
-          <t>ACIDO URICO O:P</t>
-        </is>
-      </c>
-      <c r="Q61" t="n">
-        <v>1</v>
-      </c>
-      <c r="R61" t="inlineStr"/>
-      <c r="S61" t="inlineStr"/>
-      <c r="T61" t="inlineStr"/>
-      <c r="U61" t="inlineStr"/>
-      <c r="V61" t="inlineStr"/>
-      <c r="W61" t="inlineStr"/>
-      <c r="X61" t="inlineStr"/>
-      <c r="Y61" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" s="2" t="n">
-        <v>45967.57631629148</v>
-      </c>
-      <c r="B62" t="inlineStr">
-        <is>
-          <t>812000344</t>
-        </is>
-      </c>
-      <c r="C62" t="inlineStr">
-        <is>
-          <t>11033</t>
-        </is>
-      </c>
-      <c r="D62" t="inlineStr">
-        <is>
-          <t>ESE HOSPITAL LOCAL DE MONTELIBANO</t>
-        </is>
-      </c>
-      <c r="E62" t="inlineStr">
-        <is>
-          <t>RC</t>
-        </is>
-      </c>
-      <c r="F62" t="n">
-        <v>1063316050</v>
-      </c>
-      <c r="G62" t="inlineStr">
-        <is>
-          <t>MATIAS ANDRES PEREZ QUINTERO</t>
-        </is>
-      </c>
-      <c r="H62" t="n">
-        <v>3113487853</v>
-      </c>
-      <c r="I62" t="inlineStr">
-        <is>
-          <t>3106035295</t>
-        </is>
-      </c>
-      <c r="J62" t="inlineStr">
-        <is>
-          <t>05/11/2025</t>
-        </is>
-      </c>
-      <c r="K62" t="inlineStr">
-        <is>
-          <t>Z001</t>
-        </is>
-      </c>
-      <c r="L62" t="inlineStr">
-        <is>
-          <t>PAULA ANDREA AGUAS VERGARA</t>
-        </is>
-      </c>
-      <c r="M62" t="inlineStr"/>
-      <c r="N62" t="inlineStr">
-        <is>
-          <t>PYP ENFERMERIA</t>
-        </is>
-      </c>
-      <c r="O62" t="n">
-        <v>194140</v>
-      </c>
-      <c r="P62" t="inlineStr">
-        <is>
-          <t>MÉDICO U ODONTÓLOGO GENERAL</t>
-        </is>
-      </c>
-      <c r="Q62" t="n">
-        <v>1</v>
-      </c>
-      <c r="R62" t="inlineStr"/>
-      <c r="S62" t="n">
-        <v>0</v>
-      </c>
-      <c r="T62" t="inlineStr"/>
-      <c r="U62" t="inlineStr"/>
-      <c r="V62" t="inlineStr"/>
-      <c r="W62" t="inlineStr"/>
-      <c r="X62" t="inlineStr"/>
-      <c r="Y62" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" s="2" t="n">
-        <v>45967.57631629222</v>
-      </c>
-      <c r="B63" t="inlineStr">
-        <is>
-          <t>812000344</t>
-        </is>
-      </c>
-      <c r="C63" t="inlineStr">
-        <is>
-          <t>11033</t>
-        </is>
-      </c>
-      <c r="D63" t="inlineStr">
-        <is>
-          <t>ESE HOSPITAL LOCAL DE MONTELIBANO</t>
-        </is>
-      </c>
-      <c r="E63" t="inlineStr">
-        <is>
-          <t>CC</t>
-        </is>
-      </c>
-      <c r="F63" t="n">
-        <v>9114171</v>
-      </c>
-      <c r="G63" t="inlineStr">
-        <is>
-          <t>FELIX SEGUNDO BERRIO MERCADO</t>
-        </is>
-      </c>
-      <c r="H63" t="n">
-        <v>3001900997</v>
-      </c>
-      <c r="I63" t="inlineStr">
-        <is>
-          <t>3126663905-3001900997</t>
-        </is>
-      </c>
-      <c r="J63" t="inlineStr">
-        <is>
-          <t>05/11/2025</t>
-        </is>
-      </c>
-      <c r="K63" t="inlineStr">
-        <is>
-          <t>D106</t>
-        </is>
-      </c>
-      <c r="L63" t="inlineStr">
-        <is>
-          <t>CAMILA JOHANA PACITO DIAZ</t>
-        </is>
-      </c>
-      <c r="M63" t="n">
-        <v>78</v>
-      </c>
-      <c r="N63" t="inlineStr">
-        <is>
-          <t>MEDICINA GENERAL</t>
-        </is>
-      </c>
-      <c r="O63" t="n">
-        <v>906610</v>
-      </c>
-      <c r="P63" t="inlineStr">
-        <is>
-          <t>ANTIGENO ESPECIFICO DE PROSTATA PSA</t>
-        </is>
-      </c>
-      <c r="Q63" t="n">
-        <v>1</v>
-      </c>
-      <c r="R63" t="inlineStr"/>
-      <c r="S63" t="n">
-        <v>0</v>
-      </c>
-      <c r="T63" t="inlineStr"/>
-      <c r="U63" t="inlineStr"/>
-      <c r="V63" t="inlineStr"/>
-      <c r="W63" t="inlineStr"/>
-      <c r="X63" t="inlineStr"/>
-      <c r="Y63" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" s="2" t="n">
-        <v>45967.57631629297</v>
-      </c>
-      <c r="B64" t="inlineStr">
-        <is>
-          <t>812000344</t>
-        </is>
-      </c>
-      <c r="C64" t="inlineStr">
-        <is>
-          <t>11033</t>
-        </is>
-      </c>
-      <c r="D64" t="inlineStr">
-        <is>
-          <t>ESE HOSPITAL LOCAL DE MONTELIBANO</t>
-        </is>
-      </c>
-      <c r="E64" t="inlineStr">
-        <is>
-          <t>RC</t>
-        </is>
-      </c>
-      <c r="F64" t="n">
-        <v>1063311559</v>
-      </c>
-      <c r="G64" t="inlineStr">
-        <is>
-          <t>DIDIER  CERVANTES FLOREZ</t>
-        </is>
-      </c>
-      <c r="H64" t="n">
-        <v>3113449253</v>
-      </c>
-      <c r="I64" t="inlineStr">
-        <is>
-          <t>3126969937</t>
-        </is>
-      </c>
-      <c r="J64" t="inlineStr">
-        <is>
-          <t>05/11/2025</t>
-        </is>
-      </c>
-      <c r="K64" t="inlineStr">
-        <is>
-          <t>S819</t>
-        </is>
-      </c>
-      <c r="L64" t="inlineStr">
-        <is>
-          <t>NICOLAS  MARTINEZ MACEA</t>
-        </is>
-      </c>
-      <c r="M64" t="n">
-        <v>78</v>
-      </c>
-      <c r="N64" t="inlineStr">
-        <is>
-          <t>MEDICINA GENERAL</t>
-        </is>
-      </c>
-      <c r="O64" t="n">
-        <v>865101</v>
-      </c>
-      <c r="P64" t="inlineStr">
-        <is>
-          <t>SUTURA DE HERIDA UNICA  EN AREA GENERAL</t>
-        </is>
-      </c>
-      <c r="Q64" t="n">
-        <v>1</v>
-      </c>
-      <c r="R64" t="inlineStr"/>
-      <c r="S64" t="n">
-        <v>0</v>
-      </c>
-      <c r="T64" t="inlineStr"/>
-      <c r="U64" t="inlineStr"/>
-      <c r="V64" t="inlineStr"/>
-      <c r="W64" t="inlineStr"/>
-      <c r="X64" t="inlineStr"/>
-      <c r="Y64" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>